<commit_message>
working on data iport and english translation
</commit_message>
<xml_diff>
--- a/02_work_doc/01_daten/12_component_list/componentList_oneSheet.xlsx
+++ b/02_work_doc/01_daten/12_component_list/componentList_oneSheet.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="379">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="380">
   <si>
     <t xml:space="preserve">Kategorie</t>
   </si>
@@ -68,7 +68,7 @@
     <t xml:space="preserve">Weitere Informationen / Anmerkungen</t>
   </si>
   <si>
-    <t xml:space="preserve">Quellen </t>
+    <t xml:space="preserve">Quellen</t>
   </si>
   <si>
     <t xml:space="preserve">Sensorik</t>
@@ -2612,6 +2612,9 @@
   <si>
     <t xml:space="preserve">Ecoinvent: market for display, liquid crystal, 17 inches; 
 Energieverbrauch: Digitaler CO2-Fußabdruck (GWP Herstellung auch)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quellen </t>
   </si>
   <si>
     <t xml:space="preserve">Sensor Technology</t>
@@ -3624,8 +3627,8 @@
   </sheetPr>
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="P1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P1" activeCellId="0" sqref="P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.8125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6073,7 +6076,7 @@
         <v>14</v>
       </c>
       <c r="P1" s="7" t="s">
-        <v>15</v>
+        <v>264</v>
       </c>
       <c r="Q1" s="4" t="s">
         <v>3</v>
@@ -6112,7 +6115,7 @@
         <v>14</v>
       </c>
       <c r="AC1" s="7" t="s">
-        <v>15</v>
+        <v>264</v>
       </c>
       <c r="AD1" s="4" t="s">
         <v>3</v>
@@ -6126,539 +6129,539 @@
     </row>
     <row r="2" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="61" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B2" s="61" t="s">
         <v>17</v>
       </c>
       <c r="C2" s="62" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="AB2" s="63" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="61" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B3" s="61" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="C3" s="62" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="AB3" s="61" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="61" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B4" s="61" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="C4" s="62" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="AB4" s="61" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="61" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B5" s="61" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C5" s="62" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="AB5" s="61" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="61" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B6" s="61" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C6" s="62" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="AB6" s="61" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="61" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B7" s="61" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C7" s="62" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="AB7" s="61" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="61" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B8" s="61" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="C8" s="62" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="AB8" s="61" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="61" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B9" s="61" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="C9" s="62" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="AB9" s="61" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="61" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B10" s="61" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="C10" s="62" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="AB10" s="63" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="61" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B11" s="61" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="C11" s="62" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="AB11" s="61" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="61" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B12" s="61" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C12" s="62" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="AB12" s="61" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="61" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B13" s="61" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C13" s="62" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="AB13" s="61" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="61" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B14" s="61" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="C14" s="62" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="AB14" s="61" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="61" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B15" s="61" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="C15" s="62" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="AB15" s="61" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="61" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B16" s="61" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="C16" s="62" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="AB16" s="61" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="61" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B17" s="61" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C17" s="62" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="AB17" s="61" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="61" t="s">
+        <v>290</v>
+      </c>
+      <c r="B18" s="61" t="s">
+        <v>309</v>
+      </c>
+      <c r="C18" s="62" t="s">
+        <v>310</v>
+      </c>
+      <c r="AB18" s="63" t="s">
         <v>289</v>
-      </c>
-      <c r="B18" s="61" t="s">
-        <v>308</v>
-      </c>
-      <c r="C18" s="62" t="s">
-        <v>309</v>
-      </c>
-      <c r="AB18" s="63" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="61" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B19" s="61" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="C19" s="62" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="AB19" s="61" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="61" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B20" s="61" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="C20" s="62" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="AB20" s="61" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="61" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="B21" s="61" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="C21" s="62" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="AB21" s="61" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="61" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="B22" s="61" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="C22" s="62" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="AB22" s="61" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="61" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="B23" s="61" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="C23" s="62" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="AB23" s="63" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="61" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="B24" s="61" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="C24" s="62" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="AB24" s="61" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="61" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="B25" s="61" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="C25" s="62" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="AB25" s="63" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="61" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="B26" s="61" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="C26" s="62" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="AB26" s="61" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="61" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="B27" s="61" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="C27" s="62" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="AB27" s="61" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="61" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="B28" s="61" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="C28" s="62" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="AB28" s="63" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="61" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="B29" s="61" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="C29" s="62" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="AB29" s="61" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="61" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="B30" s="61" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="C30" s="62" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="AB30" s="61" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="61" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="B31" s="61" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="C31" s="62" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="AB31" s="61" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="61" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="B32" s="61" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="C32" s="62" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="AB32" s="61" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="61" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="B33" s="61" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="C33" s="62" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="AB33" s="61" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="61" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="B34" s="61" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="C34" s="62" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="AB34" s="61" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="61" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="B35" s="61" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="C35" s="62" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="61" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="B36" s="61" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="C36" s="62" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="61" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="B37" s="61" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="C37" s="62" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="61" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="B38" s="61" t="s">
         <v>220</v>
       </c>
       <c r="C38" s="62" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="AB38" s="63" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="61" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="B39" s="61" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="C39" s="62" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="AB39" s="61" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="61" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="B40" s="61" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="C40" s="62" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="AB40" s="61" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6666,13 +6669,13 @@
         <v>239</v>
       </c>
       <c r="B41" s="61" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="C41" s="62" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="AB41" s="63" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6683,10 +6686,10 @@
         <v>243</v>
       </c>
       <c r="C42" s="62" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="AB42" s="61" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6697,10 +6700,10 @@
         <v>249</v>
       </c>
       <c r="C43" s="62" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="AB43" s="61" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6711,10 +6714,10 @@
         <v>254</v>
       </c>
       <c r="C44" s="62" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="AB44" s="61" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6725,15 +6728,15 @@
         <v>258</v>
       </c>
       <c r="C45" s="62" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="AB45" s="61" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AB46" s="63" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
debugging import of english translation into component list
</commit_message>
<xml_diff>
--- a/02_work_doc/01_daten/12_component_list/componentList_oneSheet.xlsx
+++ b/02_work_doc/01_daten/12_component_list/componentList_oneSheet.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Deutsch" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="German" sheetId="1" state="visible" r:id="rId3"/>
     <sheet name="English" sheetId="2" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
@@ -3627,8 +3627,8 @@
   </sheetPr>
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="P1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P1" activeCellId="0" sqref="P1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P3" activeCellId="0" sqref="P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.8125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
translated text fields in excel component list file, wrote tests to ensure correct functionatly of data import of translation
</commit_message>
<xml_diff>
--- a/02_work_doc/01_daten/12_component_list/componentList_oneSheet.xlsx
+++ b/02_work_doc/01_daten/12_component_list/componentList_oneSheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="German" sheetId="1" state="visible" r:id="rId3"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="378">
   <si>
     <t xml:space="preserve">Kategorie</t>
   </si>
@@ -832,74 +832,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">a</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Lüfter für kommerzielle und leichte industrielle Anwendungen, Leistungsberechnung durch Interpolation der Werte aus: https://www.dasslerventilatoren.info/contents/de/d135_WandventilatorECMotor.html, je nach Anwendung sind auch höhere Leistungen möglich 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">b</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Für die Betriebszeit wird eine tägliche Nutzung von 8-18 Uhr angenommen;
-</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">c</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Treibhausgaspotential in der Nutzungsphase wurde anhand der Emissionsfaktoren für den deutschen Strommix vom Umweltbundesamt für das Jahr 2022 berechnet  (https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke); 
-Annahme Betriebszeit: 10 h am Tag </t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve">Ökobaudat: https://oekobaudat.de/OEKOBAU.DAT/datasetdetail/process.xhtml?uuid=03f5fc6b-115b-4b86-a528-2f9311d44c9b&amp;version=20.23.050&amp;stock=OBD_2023_I&amp;lang=de</t>
   </si>
   <si>
@@ -1074,72 +1006,10 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">a</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Produtkverpackung ist inbegriffen;  für das THP wurde nur die Massenbilanz genutzt, Produktionsprozesse und deren Energieverbrauch wurden aufgrung mangelnder Daten nicht berücksichtigt; Die Berechnung erfolgte mit der CML-IA Baseline 3.08 Methode 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">b</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Treibhausgaspotential in der Nutzungsphase wurde anhand der Emissionsfaktoren für den deutschen Strommix vom Umweltbundesamt für das Jahr 2022 berechnet  (https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke); 
+    <t xml:space="preserve">&lt;sup&gt;a&lt;/sup&gt;Produtkverpackung ist inbegriffen;  für das THP wurde nur die Massenbilanz genutzt, Produktionsprozesse und deren Energieverbrauch wurden aufgrung mangelnder Daten nicht berücksichtigt; Die Berechnung erfolgte mit der CML-IA Baseline 3.08 Methode 
+&lt;sup&gt;b&lt;/sup&gt;Treibhausgaspotential in der Nutzungsphase wurde anhand der Emissionsfaktoren für den deutschen Strommix vom Umweltbundesamt für das Jahr 2022 berechnet  (https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke); 
 Die Lebensdauer des Stellmotors wird mit 15 Jahren angenommen (übliche Lebensdauer einer Dichtung);
-</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">c</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Die Betriebszeit des Stellmotors beträgt 876h </t>
-    </r>
+&lt;sup&gt;c&lt;/sup&gt;Die Betriebszeit des Stellmotors beträgt 876h </t>
   </si>
   <si>
     <t xml:space="preserve">Siemens HIT Portal: https://hit.sbt.siemens.com/RWD/app.aspx?RC=de&amp;lang=de&amp;MODULE=Catalog&amp;ACTION=ShowProduct&amp;KEY=S55150-A102</t>
@@ -1339,71 +1209,9 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">a</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Produtkverpackung ist inbegriffen; für das THP wurde nur die Massenbilanz genutzt, Produktionsprozesse und deren Energieverbrauch wurden aufgrung mangelnder Daten nicht berücksichtigt; Die Berechnung erfolgte mit der CML-IA Baseline 3.08 Methode 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">b</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Treibhausgaspotential in der Nutzungsphase wurde anhand der Emissionsfaktoren für den deutschen Strommix vom Umweltbundesamt für das Jahr 2022 berechnet  (https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke); 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">c</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Es wird eine Betriebszeit von 16h am Tag angenommen (durchschnittliche Wachzeit)</t>
-    </r>
+    <t xml:space="preserve">&lt;sup&gt;a&lt;/sup&gt;Produtkverpackung ist inbegriffen; für das THP wurde nur die Massenbilanz genutzt, Produktionsprozesse und deren Energieverbrauch wurden aufgrung mangelnder Daten nicht berücksichtigt; Die Berechnung erfolgte mit der CML-IA Baseline 3.08 Methode 
+&lt;sup&gt;b&lt;/sup&gt;Treibhausgaspotential in der Nutzungsphase wurde anhand der Emissionsfaktoren für den deutschen Strommix vom Umweltbundesamt für das Jahr 2022 berechnet  (https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke); 
+&lt;sup&gt;c&lt;/sup&gt;Es wird eine Betriebszeit von 16h am Tag angenommen (durchschnittliche Wachzeit)</t>
   </si>
   <si>
     <t xml:space="preserve">Siemens HIT Portal: https://hit.sbt.siemens.com/RWD/app.aspx?RC=de&amp;lang=de&amp;MODULE=Catalog&amp;ACTION=ShowProduct&amp;KEY=5WG1526-4DB23</t>
@@ -2305,108 +2113,63 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">a</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Produtkverpackung ist inbegriffen;  für das THP wurde nur die Massenbilanz genutzt, Produktionsprozesse und deren Energieverbrauch wurden aufgrung mangelnder Daten nicht berücksichtigt; Die Berechnung erfolgte mit der CML-IA Baseline 3.08 Methode 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">b</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Treibhausgaspotential in der Nutzungsphase wurde anhand der Emissionsfaktoren für den deutschen Strommix vom Umweltbundesamt für das Jahr 2022 berechnet  (https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke); </t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Siemens HIT Portal: https://hit.sbt.siemens.com/RWD/app.aspx?RC=de&amp;lang=de&amp;MODULE=Catalog&amp;ACTION=ShowProduct&amp;KEY=5WG1125-1AB22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BUS-System: KNX Zusatzspannungsversorgung</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Die Zusatzspannungsversorgung erzeugt die für das KNX System erforderliche Spannung und ist nur erforderlich, wenn im Systen an einer Komponente die Spannung unter 21 V fällt. Der Bemessungsstrom liet bei 80 mA</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">16,98</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">a</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">436,25</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">b</t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve">&lt;sup&gt;a&lt;/sup&gt;Produtkverpackung ist inbegriffen;  für das THP wurde nur die Massenbilanz genutzt, Produktionsprozesse und deren Energieverbrauch wurden aufgrung mangelnder Daten nicht berücksichtigt; Die Berechnung erfolgte mit der CML-IA Baseline 3.08 Methode 
 &lt;sup&gt;b&lt;/sup&gt;Treibhausgaspotential in der Nutzungsphase wurde anhand der Emissionsfaktoren für den deutschen Strommix vom Umweltbundesamt für das Jahr 2022 berechnet  (https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke); </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Siemens HIT Portal: https://hit.sbt.siemens.com/RWD/app.aspx?RC=de&amp;lang=de&amp;MODULE=Catalog&amp;ACTION=ShowProduct&amp;KEY=5WG1125-1AB22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BUS-System: KNX Zusatzspannungsversorgung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Die Zusatzspannungsversorgung erzeugt die für das KNX System erforderliche Spannung und ist nur erforderlich, wenn im Systen an einer Komponente die Spannung unter 21 V fällt. Der Bemessungsstrom liet bei 80 mA</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">16,98</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">a</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">436,25</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">b</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Siemens HIT Portal: https://hit.sbt.siemens.com/RWD/app.aspx?RC=de&amp;lang=de&amp;MODULE=Catalog&amp;ACTION=ShowProduct&amp;KEY=5WG1125-4AB23</t>
@@ -2623,9 +2386,9 @@
     <t xml:space="preserve">CO2 measuring element based on non-dispersive infrared (NDIR) absorption measurement. Used in ventilation and air conditioning systems to optimize comfort and energy consumption through demand-controlled ventilation and to measure CO2 concentration.</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;sup&gt;a&lt;/sup&gt; Product packaging is included; for the THP, only the mass balance was used, and production processes along with their energy consumption were not considered due to a lack of data; The calculation was performed using the CML-IA Baseline 3.08 method.
-&lt;sup&gt;b&lt;/sup&gt; The greenhouse gas potential during the usage phase was calculated based on emission factors for the German electricity mix from the Federal Environment Agency for the year 2022 (https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke);
-&lt;sup&gt;c&lt;/sup&gt; Assumed operating time: 24h/day</t>
+    <t xml:space="preserve">&lt;sup&gt;a&lt;/sup&gt;Packaging is included; for the THP, only the mass balance was used, production processes and their energy consumption were not considered due to a lack of data; The calculation was performed using the CML-IA Baseline 3.08 method.
+&lt;sup&gt;b&lt;/sup&gt;Greenhouse gas potential during the usage phase was calculated based on the emission factors for the German electricity mix from the Federal Environment Agency for the year 2022 (https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke);
+&lt;sup&gt;c&lt;/sup&gt;Assumption of operating time: 24h/day.</t>
   </si>
   <si>
     <t xml:space="preserve">Temperature Sensor</t>
@@ -2634,9 +2397,7 @@
     <t xml:space="preserve">Temperature measuring device with a small display for measuring indoor temperature. Connection options to a BUS system for power supply and communication.</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;sup&gt;a&lt;/sup&gt; Product packaging is included;
-&lt;sup&gt;b&lt;/sup&gt; Operating time: 100% load rate
-</t>
+    <t xml:space="preserve">&lt;sup&gt;a&lt;/sup&gt;Product packaging is included;&lt;sup&gt;b&lt;/sup&gt;Operating time: 100% load rate.</t>
   </si>
   <si>
     <t xml:space="preserve">Wireless Temperature Sensor</t>
@@ -2645,325 +2406,810 @@
     <t xml:space="preserve">Sensor for continuous temperature measurement with wireless transmission to a concentrator. The operating energy is harvested from the electromagnetic energy around the current transmission line. The component offers connection options for up to three temperature probes.</t>
   </si>
   <si>
+    <t xml:space="preserve">Humidity Sensor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Humidity sensor module for use in HVAC systems to measure relative humidity and temperature with high accuracy and short response time. Measures humidity from 0-100%. Includes connections for power supply and BUS system via cable.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">&lt;sup&gt;a&lt;/sup&gt;Product packaging is included; for the THP, only the mass balance was used, production processes and their energy consumption were not considered due to a lack of data; the calculation was performed using the CML-IA Baseline 3.08 method.
+&lt;sup&gt;b&lt;/sup&gt;Greenhouse gas potential during the usage phase was calculated based on the emission factors for the German electricity mix from the Federal Environment Agency for the year 2022 (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">);
+&lt;sup&gt;c&lt;/sup&gt;Assumption of operating time: 24h/day.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Presence Detector</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Presence detector that detects the movement of people in a room to control indoor lighting.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;sup&gt;a&lt;/sup&gt;Packaging is included, European electricity mix;
+&lt;sup&gt;b&lt;/sup&gt;Operating time: Assumption = 30% active; 70% passive.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Light Sensor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sunlight sensor used as a probe in HVAC systems where solar radiation compensation is planned. The probe uses a solar cell to detect sunlight and generates a radiation-dependent current that is evaluated by the sensor.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;sup&gt;a&lt;/sup&gt;Product packaging is included; for the THP, only the mass balance was used, production processes and their energy consumption were not considered due to a lack of data; the calculation was performed using the CML-IA Baseline 3.08 method.
+&lt;sup&gt;b&lt;/sup&gt;The light sensor is equipped with a solar module and requires no external energy during the usage phase;
+&lt;sup&gt;c&lt;/sup&gt;An operating time of 12 hours per day is assumed (average daylight time per year).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Water Meter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Conventional water meter for physical measurement of cold/hot water consumption. The meter consists of a flow element, a counter, and a display. Flow rate: 4 m³/h.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Heat Meter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ultrasonic heat and cooling energy meter for measuring flow and energy in heating or cooling circuits. Flow rate: 25 m³/h.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">&lt;sup&gt;a&lt;/sup&gt;Product packaging is included; for the THP, only the mass balance was used, production processes and their energy consumption were not considered due to a lack of data; the calculation was performed using the CML-IA Baseline 3.08 method.
+&lt;sup&gt;b&lt;/sup&gt;Greenhouse gas potential during the usage phase was calculated based on the emission factors for the German electricity mix from the Federal Environment Agency for the year 2022 (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">);
+&lt;sup&gt;c&lt;/sup&gt;Assumed operating time: 24h/day.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Flow Meter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ultrasonic flow sensor with a maximum flow rate of 12 m³/h (volume flow meter).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;sup&gt;a&lt;/sup&gt;Product packaging is included; for the THP, only the mass balance was used, production processes and their energy consumption were not considered due to a lack of data; the calculation was performed using the CML-IA Baseline 3.08 method.
+&lt;sup&gt;b&lt;/sup&gt;No data is available for the electrical power, so no greenhouse gas potential could be calculated for the usage phase;
+&lt;sup&gt;c&lt;/sup&gt;Assumed operating time: 24h/day.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actuator Technology</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Small Fan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Central ventilation system for supply or exhaust air with a capacity of 5000 m³/h. It is a fan installed on the roof or beside the building, housed in a galvanized steel casing.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">&lt;sup&gt;a&lt;/sup&gt;Fan for commercial and light industrial applications, performance calculation by interpolating the values from: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">https://www.dasslerventilatoren.info/contents/de/d135_WandventilatorECMotor.html</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">; higher power outputs are possible depending on the application.
+&lt;sup&gt;b&lt;/sup&gt;A daily usage time from 8 AM to 6 PM is assumed.
+&lt;sup&gt;c&lt;/sup&gt;Greenhouse gas potential during the usage phase was calculated based on the emission factors for the German electricity mix from the Federal Environment Agency for the year 2022 (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">);
+Assumed operating time: 10 hours per day.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Medium Fan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Central ventilation system for supply or exhaust air with a capacity of 10,000 m³/h. It is a fan installed on the roof or beside the building, housed in a galvanized steel casing.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">&lt;sup&gt;a&lt;/sup&gt;Fan for commercial and light industrial applications, performance calculated by interpolating the values from: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">https://www.dasslerventilatoren.info/contents/de/d135_WandventilatorECMotor.html</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">; higher power outputs are possible depending on the application.
+&lt;sup&gt;b&lt;/sup&gt;A daily usage time from 8 AM to 6 PM is assumed.
+&lt;sup&gt;c&lt;/sup&gt;Greenhouse gas potential during the usage phase was calculated based on the emission factors for the German electricity mix from the Federal Environment Agency for the year 2022 (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">);
+Assumed operating time: 10 hours per day.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Large Fan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Central ventilation system for supply or exhaust air with a capacity of 30,000 m³/h. It is a fan installed on the roof or beside the building, housed in a galvanized steel casing.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Volume Flow Controller</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Electronic volume flow controller for installation in air ducts for supply and exhaust air in HVAC systems. The control method uses differential pressure and flap position for volume flow measurement and control. Static pressure control range: 20-1000 Pa; allowable airspeed: 12 m/s; volume flow range: 34-5430 m³/h.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;sup&gt;b&lt;/sup&gt;Greenhouse gas potential during the usage phase is calculated by multiplying the annual value by the lifespan.
+&lt;sup&gt;a&lt;/sup&gt;Operating time: 91.25 hours per year in operation, otherwise idle.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Circulation Pump</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Circulation pump with a power rating of 50-250 W for heating systems.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">&lt;sup&gt;b&lt;/sup&gt;Greenhouse gas potential during the usage phase was calculated based on the emission factors for the German electricity mix from the Federal Environment Agency for the year 2022 (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">);
+&lt;sup&gt;a&lt;/sup&gt;Assumed operating time: 3,000 hours per year (range: 2,000 to 4,000 hours);
+&lt;sup&gt;c&lt;/sup&gt;The circulation pump has a power rating of 50-250W; for the calculation, an effective power of 150W is assumed.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Small Electric Valve Actuator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Small electric valve actuator for controlling water-side regulation of hot and cooling water in HVAC systems. Automatic detection of valve stroke. Includes manual adjuster and position indicator.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">&lt;sup&gt;a&lt;/sup&gt;Product packaging is included; for the THP, only the mass balance was used, production processes and their energy consumption were not considered due to a lack of data; the calculation was performed using the CML-IA Baseline 3.08 method.
+&lt;sup&gt;b&lt;/sup&gt;Greenhouse gas potential during the usage phase was calculated based on the emission factors for the German electricity mix from the Federal Environment Agency for the year 2022 (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">);
+The lifespan of the actuator is assumed to be 15 years (typical lifespan of a seal);
+&lt;sup&gt;c&lt;/sup&gt;The operating time of the actuator is 876 hours.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Large Electric Valve Actuator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Electric actuator for operating two-way and three-way valves with a 20mm stroke as control and shut-off devices in HVAC systems. Includes manual adjuster, position, and status indicator.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">&lt;sup&gt;a&lt;/sup&gt;Product packaging is included; for the THP, only the mass balance was used, production processes and their energy consumption were not considered due to a lack of data; the calculation was performed using the CML-IA Baseline 3.08 method.
+&lt;sup&gt;b&lt;/sup&gt;Greenhouse gas potential during the usage phase was calculated based on the emission factors for the German electricity mix from the Federal Environment Agency for the year 2022 (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">).</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">BUS System: KNX Sunshade Actuator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sunshade actuator used to control blinds, shutters, awnings, or ventilation flap drives.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;sup&gt;a&lt;/sup&gt;Product packaging is included; for the THP, only the mass balance was used, production processes and their energy consumption were not considered due to a lack of data; the calculation was performed using the CML-IA Baseline 3.08 method.
+&lt;sup&gt;b&lt;/sup&gt;Greenhouse gas potential during the usage phase was calculated based on the emission factors for the German electricity mix from the Federal Environment Agency for the year 2022 (https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke).
+&lt;sup&gt;c&lt;/sup&gt;An operating time of 12 hours per day is assumed (average daylight time per year).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BUS System: KNX Switch/Dimmer Actuator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Switch/dimmer actuator used for switching, dimming, and scene control (e.g., LED) in building automation. Device control is via KNX.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">&lt;sup&gt;a&lt;/sup&gt;Product packaging is included; for the THP, only the mass balance was used, production processes and their energy consumption were not considered due to a lack of data; the calculation was performed using the CML-IA Baseline 3.08 method.
+&lt;sup&gt;b&lt;/sup&gt;Greenhouse gas potential during the usage phase was calculated based on the emission factors for the German electricity mix from the Federal Environment Agency for the year 2022 (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">).
+&lt;sup&gt;c&lt;/sup&gt;An operating time of 16 hours per day is assumed (average wake time).</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">BUS System: KNX Thermo Actuator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thermo actuator with 2 outputs for controlling electrothermal actuators in heating or cooling systems.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">&lt;sup&gt;a&lt;/sup&gt;Product packaging is included; for the THP, only the mass balance was used, production processes and their energy consumption were not considered due to a lack of data; the calculation was performed using the CML-IA Baseline 3.08 method.
+&lt;sup&gt;b&lt;/sup&gt;Greenhouse gas potential during the usage phase was calculated based on the emission factors for the German electricity mix from the Federal Environment Agency for the year 2022 (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">).
+&lt;sup&gt;c&lt;/sup&gt;An operating time of 24 hours per day is assumed.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Signal Processing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Communication Interface</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USB adapter that enables communication via the Zigbee protocol by connecting to a server or IP controller.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;sup&gt;a&lt;/sup&gt;Product packaging is included.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Connection Cable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Generic cable from the Ecoinvent database. Components: 66% copper, 34% insulator.</t>
+  </si>
+  <si>
     <t xml:space="preserve">&lt;sup&gt;c&lt;/sup&gt; Assumed operating time: 24 hours/day.</t>
   </si>
   <si>
-    <t xml:space="preserve">Humidity Sensor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Humidity sensor module for use in HVAC systems to measure relative humidity and temperature with high accuracy and short response time. Measures humidity from 0-100%. Includes connections for power supply and BUS system via cable.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;sup&gt;a&lt;/sup&gt; Product packaging is included;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Presence Detector</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Presence detector that detects the movement of people in a room to control indoor lighting.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;sup&gt;b&lt;/sup&gt; Operating time: 100% load rate.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Light Sensor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sunlight sensor used as a probe in HVAC systems where solar radiation compensation is planned. The probe uses a solar cell to detect sunlight and generates a radiation-dependent current that is evaluated by the sensor.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Water Meter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Conventional water meter for physical measurement of cold/hot water consumption. The meter consists of a flow element, a counter, and a display. Flow rate: 4 m³/h.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Heat Meter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ultrasonic heat and cooling energy meter for measuring flow and energy in heating or cooling circuits. Flow rate: 25 m³/h.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;sup&gt;a&lt;/sup&gt; Product packaging is included; for the LCA, only the mass balance was used, production processes and their energy consumption were not considered due to a lack of data; the calculation was performed using the CML-IA Baseline 3.08 method.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Flow Meter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ultrasonic flow sensor with a maximum flow rate of 12 m³/h (volume flow meter).</t>
+    <t xml:space="preserve">Analog/Digital Converter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Microchip for converting analog to digital signals, mounted on a circuit board.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;sup&gt;a&lt;/sup&gt;For the THP, only the mass balance was used; production processes and their energy consumption were not considered due to a lack of data; the calculation was performed using the CML-IA Baseline 3.08 method.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Circuit Board</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 kg of a populated circuit board with electronic components such as capacitors, resistors, etc., already soldered onto the board. The solder and surface used for mounting the components are lead-free.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;sup&gt;a&lt;/sup&gt;An operating time of 24 hours per day is assumed.
+&lt;sup&gt;b&lt;/sup&gt;The electricity consumption and greenhouse gas potential during the usage phase are not considered, as they are highly dependent on individual circumstances.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data Logger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data logger that allows a master device to access data collected by connected slave devices. Communication is possible via various bus systems, including wireless.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BUS System: KNX BACnet Interface</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Interface between KNX and BACnet. KNX communication objects are translated into BACnet objects and can communicate within a BACnet system.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BUS System: KNX DALI Interface</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Interface between KNX and DALI. Up to 64 DALI actuators and additional sensors can be connected per channel.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">&lt;sup&gt;a&lt;/sup&gt;Product packaging is included; for the THP, only the mass balance was used, production processes and their energy consumption were not considered due to a lack of data; the calculation was performed using the CML-IA Baseline 3.08 method.
+&lt;sup&gt;b&lt;/sup&gt;Greenhouse gas potential during the usage phase was calculated based on the emission factors for the German electricity mix from the Federal Environment Agency for the year 2022 (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">).
+&lt;sup&gt;c&lt;/sup&gt;It is assumed that the BACnet and DALI interfaces have similar energy consumption values.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">BUS System: KNX IP Router Interface</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IP router that connects KNX lines via data networks using the Internet Protocol and the KNXnet/IP standard. This device also allows bus access from a PC or other data processing devices.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;sup&gt;a&lt;/sup&gt;Product packaging is included; for the THP, only the mass balance was used, production processes and their energy consumption were not considered due to a lack of data; the calculation was performed using the CML-IA Baseline 3.08 method.
+&lt;sup&gt;b&lt;/sup&gt;Greenhouse gas potential during the usage phase was calculated based on the emission factors for the German electricity mix from the Federal Environment Agency for the year 2022 (https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BUS System: KNX IP Control Center</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Web server component integrated for operation, monitoring, and programming of KNX systems. Standard web browsers can display and visually represent control pages. The component provides an interface to KNX installations via IP data networks.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BUS System: KNX Web Server</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Web server enabling remote control and monitoring of systems via web and smartphone app.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">&lt;sup&gt;a&lt;/sup&gt;Product packaging is included; for the THP, only the mass balance was used. Production processes and their energy consumption were not considered due to a lack of data; the calculation was performed using the CML-IA Baseline 3.08 method.
+&lt;sup&gt;b&lt;/sup&gt;Greenhouse gas potential during the usage phase was calculated based on the emission factors for the German electricity mix from the Federal Environment Agency for the year 2022 (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">).</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">BUS System: KNX Repeater</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Line coupler used for coupling a line to a main line, area coupler for coupling a main line to the area line, or line amplifier (repeater) for coupling two segments of the same line.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BUS System: KNX Input Device</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Binary input device with 8 inputs for potential-free contacts for processing binary signals (e.g., switches, push buttons, detectors).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BUS System: KNX Output Device</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Output unit with control functions (switching with status feedback, logic gates, central switching, timed switching, and night mode), override functions (manual override ON, permanent OFF, locking, central override, and forced guidance), and diagnostic functions (switch cycle count with limit monitoring, operating hour count with limit monitoring, and status feedback).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Infrastructure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Power Line</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 meter of a three-wire cable from the Ecoinvent database. 1 kV low voltage cable with copper wire sheath for distribution networks and industry.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Water Line</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Process considering the production of a drinking water pipe made of stainless steel (cold-rolled). The process includes bending the steel sheet, welding the seam, all necessary processes, and the total energy expenditure.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Air Line</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ventilation duct made of galvanized steel sheet for ventilation or air conditioning without insulation.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Power Meter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Household Ferraris-type electricity meter.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">&lt;sup&gt;a&lt;/sup&gt;An operating time of 24 hours per day was assumed.
+&lt;sup&gt;b&lt;/sup&gt;Greenhouse gas potential during the usage phase was calculated based on the emission factors for the German electricity mix from the Federal Environment Agency for the year 2022 (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">).
+&lt;sup&gt;c&lt;/sup&gt;For the THP, only the mass balance was used. Production processes and their energy consumption were not considered due to a lack of data; the calculation was performed using the CML-IA Baseline 3.08 method.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Smart meter electricity meter.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;sup&gt;a&lt;/sup&gt;An operating time of 24 hours per day was assumed.
+&lt;sup&gt;b&lt;/sup&gt;Greenhouse gas potential during the usage phase was calculated based on the emission factors for the German electricity mix from the Federal Environment Agency for the year 2022 (https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke).
+&lt;sup&gt;c&lt;/sup&gt;For the THP, only the mass balance was used. Production processes and their energy consumption were not considered due to a lack of data; the calculation was performed using the CML-IA Baseline 3.08 method.
+&lt;sup&gt;d&lt;/sup&gt;For the average power consumption, the upper value of the manufacturer’s specification in Source [2] was used.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BUS System: KNX Power Supply</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Component providing the necessary basic voltage for the KNX system. Rated current: 640 mA.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BUS System: KNX Auxiliary Power Supply</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Auxiliary power supply providing the necessary voltage for the KNX system, required only if the voltage in a component drops below 21 V. Rated current: 80 mA.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LAN Cable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 meter of typical network cable of category 5 (data cable up to 100 Mbit/s) without connectors.</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;sup&gt;b&lt;/sup&gt; Greenhouse gas potential during the usage phase was calculated based on emission factors for the German electricity mix provided by the Federal Environment Agency for the year 2022 (https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke);</t>
   </si>
   <si>
-    <t xml:space="preserve">Actuator Technology</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Small Fan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Central ventilation system for supply or exhaust air with a capacity of 5000 m³/h. It is a fan installed on the roof or beside the building, housed in a galvanized steel casing.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Medium Fan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Central ventilation system for supply or exhaust air with a capacity of 10,000 m³/h. It is a fan installed on the roof or beside the building, housed in a galvanized steel casing.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;sup&gt;a&lt;/sup&gt; Packaging is included, European electricity mix;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Large Fan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Central ventilation system for supply or exhaust air with a capacity of 30,000 m³/h. It is a fan installed on the roof or beside the building, housed in a galvanized steel casing.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;sup&gt;b&lt;/sup&gt; Operating time: Assumption = 30% active; 70% passive.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Volume Flow Controller</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Electronic volume flow controller for installation in air ducts for supply and exhaust air in HVAC systems. The control method uses differential pressure and flap position for volume flow measurement and control. Static pressure control range: 20-1000 Pa; allowable airspeed: 12 m/s; volume flow range: 34-5430 m³/h.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Circulation Pump</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Circulation pump with a power rating of 50-250 W for heating systems.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;sup&gt;b&lt;/sup&gt; The light sensor is equipped with a solar module and does not require external energy during the usage phase;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Small Electric Valve Actuator</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Small electric valve actuator for controlling water-side regulation of hot and cooling water in HVAC systems. Automatic detection of valve stroke. Includes manual adjuster and position indicator.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;sup&gt;c&lt;/sup&gt; An operating time of 12 hours per day is assumed (average daylight hours per year).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Large Electric Valve Actuator</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Electric actuator for operating two-way and three-way valves with a 20mm stroke as control and shut-off devices in HVAC systems. Includes manual adjuster, position, and status indicator.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BUS System: KNX Sunshade Actuator</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sunshade actuator used to control blinds, shutters, awnings, or ventilation flap drives.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BUS System: KNX Switch/Dimmer Actuator</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Switch/dimmer actuator used for switching, dimming, and scene control (e.g., LED) in building automation. Device control is via KNX.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BUS System: KNX Thermo Actuator</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thermo actuator with 2 outputs for controlling electrothermal actuators in heating or cooling systems.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Signal Processing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Communication Interface</t>
-  </si>
-  <si>
-    <t xml:space="preserve">USB adapter that enables communication via the Zigbee protocol by connecting to a server or IP controller.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;sup&gt;b&lt;/sup&gt; No data on electrical power is available, so no greenhouse potential could be calculated for the usage phase;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Connection Cable</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Generic cable from the Ecoinvent database. Components: 66% copper, 34% insulator.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Analog/Digital Converter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Microchip for converting analog to digital signals, mounted on a circuit board.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;sup&gt;a&lt;/sup&gt; Fan for commercial and light industrial applications, performance calculation by interpolation of values from: https://www.dasslerventilatoren.info/contents/de/d135_WandventilatorECMotor.html, depending on the application, higher performances are also possible.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Circuit Board</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 kg of a populated circuit board with electronic components such as capacitors, resistors, etc., already soldered onto the board. The solder and surface used for mounting the components are lead-free.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;sup&gt;b&lt;/sup&gt; For the operating time, a daily usage from 8 AM to 6 PM is assumed;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Data Logger</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Data logger that allows a master device to access data collected by connected slave devices. Communication is possible via various bus systems, including wireless.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;sup&gt;c&lt;/sup&gt; Greenhouse gas potential during the usage phase was calculated based on emission factors for the German electricity mix provided by the Federal Environment Agency for the year 2022 (https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke); Assumed operating time: 10 hours per day.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BUS System: KNX BACnet Interface</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Interface between KNX and BACnet. KNX communication objects are translated into BACnet objects and can communicate within a BACnet system.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;sup&gt;a&lt;/sup&gt; Greenhouse gas potential during the usage phase is calculated based on the value per year multiplied by the lifespan;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BUS System: KNX DALI Interface</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Interface between KNX and DALI. Up to 64 DALI actuators and additional sensors can be connected per channel.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;sup&gt;b&lt;/sup&gt; Operating time: 91.25 hours per year in regulation, otherwise dormant.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BUS System: KNX IP Router Interface</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IP router that connects KNX lines via data networks using the Internet Protocol and the KNXnet/IP standard. This device also allows bus access from a PC or other data processing devices.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;sup&gt;a&lt;/sup&gt; Greenhouse gas potential during the usage phase was calculated based on emission factors for the German electricity mix provided by the Federal Environment Agency for the year 2022 (https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke);</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BUS System: KNX IP Control Center</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Web server component integrated for operation, monitoring, and programming of KNX systems. Standard web browsers can display and visually represent control pages. The component provides an interface to KNX installations via IP data networks.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;sup&gt;b&lt;/sup&gt; Assumed operating time: 3000 hours per year (2000 hours-4000 hours);</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BUS System: KNX Web Server</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Web server enabling remote control and monitoring of systems via web and smartphone app.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;sup&gt;c&lt;/sup&gt; The circulation pump has a power rating of 50-250W, for the calculation, an effective power of 150W is assumed.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BUS System: KNX Repeater</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Line coupler used for coupling a line to a main line, area coupler for coupling a main line to the area line, or line amplifier (repeater) for coupling two segments of the same line.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BUS System: KNX Input Device</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Binary input device with 8 inputs for potential-free contacts for processing binary signals (e.g., switches, push buttons, detectors).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;sup&gt;b&lt;/sup&gt; The lifetime of the actuator is assumed to be 15 years (typical lifespan of a seal);</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BUS System: KNX Output Device</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Output unit with control functions (switching with status feedback, logic gates, central switching, timed switching, and night mode), override functions (manual override ON, permanent OFF, locking, central override, and forced guidance), and diagnostic functions (switch cycle count with limit monitoring, operating hour count with limit monitoring, and status feedback).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;sup&gt;c&lt;/sup&gt; The operating time of the actuator is 876 hours.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Infrastructure</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Power Line</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 meter of a three-wire cable from the Ecoinvent database. 1 kV low voltage cable with copper wire sheath for distribution networks and industry.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Water Line</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Process considering the production of a drinking water pipe made of stainless steel (cold-rolled). The process includes bending the steel sheet, welding the seam, all necessary processes, and the total energy expenditure.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Air Line</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ventilation duct made of galvanized steel sheet for ventilation or air conditioning without insulation.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Power Meter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Household Ferraris-type electricity meter.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Smart meter electricity meter.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BUS System: KNX Power Supply</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Component providing the necessary basic voltage for the KNX system. Rated current: 640 mA.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;sup&gt;c&lt;/sup&gt; It is assumed that the BACnet and DALI interfaces have similar energy consumption values.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BUS System: KNX Auxiliary Power Supply</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Auxiliary power supply providing the necessary voltage for the KNX system, required only if the voltage in a component drops below 21 V. Rated current: 80 mA.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;sup&gt;a&lt;/sup&gt; A 24-hour/day operating time is assumed;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LAN Cable</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 meter of typical network cable of category 5 (data cable up to 100 Mbit/s) without connectors.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Router for connecting to the internet from the Ecoinvent database. The product represents a Cisco Service Router 1800 Series with a maximum data rate of 100 Mbit/s and a realistic data rate of 25 Mbit/s.</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;sup&gt;c&lt;/sup&gt; for the LCA, only the mass balance was used, production processes and their energy consumption were not considered due to a lack of data; the calculation was performed using the CML-IA Baseline 3.08 method.</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">&lt;sup&gt;b&lt;/sup&gt;Greenhouse gas potential during the usage phase was calculated based on the emission factors for the German electricity mix from the Federal Environment Agency for the year 2022 (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">).
+&lt;sup&gt;a&lt;/sup&gt;An operating time of 24 hours per day was assumed.
+&lt;sup&gt;c&lt;/sup&gt;The router's power consumption is 105W with an effective data transfer rate of 25 Mbit/s.</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Desktop computer without monitor from the Ecoinvent database. The product represents a typical desktop computer with a Pentium 4, 2000 MHz processor speed, 40 GB RAM HDD, and 512 GB storage capacity.</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;sup&gt;d&lt;/sup&gt; For the average power consumption, the upper value of the manufacturer's specification in Source [2] was used.</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">&lt;sup&gt;a&lt;/sup&gt;An operating time of 24 hours per day is assumed for the measurement computer in its function.
+&lt;sup&gt;b&lt;/sup&gt;Greenhouse gas potential during the usage phase was calculated based on the emission factors for the German electricity mix from the Federal Environment Agency for the year 2022 (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">).</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Laptop computer from the Ecoinvent database. The product represents a typical laptop with a Pentium 3, 600 MHz processor speed, 10 GB RAM, 128 GB storage capacity, and a 12.1-inch screen.</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;sup&gt;a&lt;/sup&gt; The router's power consumption is 105W at an effective data transmission rate of 25 Mbit/s.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Thin-film transistor LCD display for a desktop computer. The product includes all display components, including electronics, frame, and energy consumption during manufacturing.</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;sup&gt;b&lt;/sup&gt; In its function as a measurement computer, a 24-hour/day operating time is assumed;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;sup&gt;c&lt;/sup&gt; Greenhouse gas potential during the usage phase was calculated based on emission factors for the German electricity mix provided by the Federal Environment Agency for the year 2022 (https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke).</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">&lt;sup&gt;b&lt;/sup&gt;Greenhouse gas potential during the usage phase was calculated based on the emission factors for the German electricity mix from the Federal Environment Agency for the year 2022 (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">).
+&lt;sup&gt;a&lt;/sup&gt;The monitor of the measurement computer is used only during working hours: 250 days/year * 8 hours = 2000 hours.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -2975,7 +3221,7 @@
     <numFmt numFmtId="165" formatCode="0.00"/>
     <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="13">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -3039,6 +3285,24 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -3338,14 +3602,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3439,6 +3695,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3627,8 +3891,8 @@
   </sheetPr>
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P3" activeCellId="0" sqref="P3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="N36" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O45" activeCellId="0" sqref="O45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.8125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4310,11 +4574,11 @@
       <c r="N13" s="36" t="n">
         <v>-398.618</v>
       </c>
-      <c r="O13" s="38" t="s">
+      <c r="O13" s="37" t="s">
+        <v>79</v>
+      </c>
+      <c r="P13" s="31" t="s">
         <v>91</v>
-      </c>
-      <c r="P13" s="31" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4322,10 +4586,10 @@
         <v>73</v>
       </c>
       <c r="B14" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="C14" s="23" t="s">
         <v>93</v>
-      </c>
-      <c r="C14" s="23" t="s">
-        <v>94</v>
       </c>
       <c r="D14" s="24" t="n">
         <v>4.47125</v>
@@ -4356,16 +4620,16 @@
         <v>19.11695</v>
       </c>
       <c r="M14" s="28" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="N14" s="29" t="n">
         <v>-2.84496</v>
       </c>
       <c r="O14" s="30" t="s">
+        <v>95</v>
+      </c>
+      <c r="P14" s="31" t="s">
         <v>96</v>
-      </c>
-      <c r="P14" s="31" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4373,10 +4637,10 @@
         <v>73</v>
       </c>
       <c r="B15" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="C15" s="23" t="s">
         <v>98</v>
-      </c>
-      <c r="C15" s="23" t="s">
-        <v>99</v>
       </c>
       <c r="D15" s="24" t="n">
         <v>450</v>
@@ -4395,13 +4659,13 @@
         <v>10</v>
       </c>
       <c r="I15" s="28" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J15" s="27" t="s">
         <v>19</v>
       </c>
       <c r="K15" s="33" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L15" s="32" t="n">
         <v>24.94063</v>
@@ -4414,10 +4678,10 @@
         <v>-3.16639</v>
       </c>
       <c r="O15" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="P15" s="31" t="s">
         <v>102</v>
-      </c>
-      <c r="P15" s="31" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4425,10 +4689,10 @@
         <v>73</v>
       </c>
       <c r="B16" s="22" t="s">
+        <v>103</v>
+      </c>
+      <c r="C16" s="23" t="s">
         <v>104</v>
-      </c>
-      <c r="C16" s="23" t="s">
-        <v>105</v>
       </c>
       <c r="D16" s="24" t="n">
         <v>0.6</v>
@@ -4453,22 +4717,22 @@
         <v>19</v>
       </c>
       <c r="K16" s="28" t="s">
+        <v>105</v>
+      </c>
+      <c r="L16" s="28" t="s">
         <v>106</v>
       </c>
-      <c r="L16" s="28" t="s">
+      <c r="M16" s="28" t="s">
         <v>107</v>
-      </c>
-      <c r="M16" s="28" t="s">
-        <v>108</v>
       </c>
       <c r="N16" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="O16" s="39" t="s">
+      <c r="O16" s="30" t="s">
+        <v>108</v>
+      </c>
+      <c r="P16" s="31" t="s">
         <v>109</v>
-      </c>
-      <c r="P16" s="31" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4476,10 +4740,10 @@
         <v>73</v>
       </c>
       <c r="B17" s="22" t="s">
+        <v>110</v>
+      </c>
+      <c r="C17" s="23" t="s">
         <v>111</v>
-      </c>
-      <c r="C17" s="23" t="s">
-        <v>112</v>
       </c>
       <c r="D17" s="24" t="n">
         <v>4</v>
@@ -4507,19 +4771,19 @@
         <v>876</v>
       </c>
       <c r="L17" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="M17" s="28" t="s">
         <v>113</v>
-      </c>
-      <c r="M17" s="28" t="s">
-        <v>114</v>
       </c>
       <c r="N17" s="29" t="s">
         <v>23</v>
       </c>
       <c r="O17" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="P17" s="31" t="s">
         <v>115</v>
-      </c>
-      <c r="P17" s="31" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4527,10 +4791,10 @@
         <v>73</v>
       </c>
       <c r="B18" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="C18" s="23" t="s">
         <v>117</v>
-      </c>
-      <c r="C18" s="23" t="s">
-        <v>118</v>
       </c>
       <c r="D18" s="24" t="n">
         <v>13.14</v>
@@ -4558,19 +4822,19 @@
         <v>52</v>
       </c>
       <c r="L18" s="28" t="s">
+        <v>118</v>
+      </c>
+      <c r="M18" s="28" t="s">
         <v>119</v>
-      </c>
-      <c r="M18" s="28" t="s">
-        <v>120</v>
       </c>
       <c r="N18" s="29" t="s">
         <v>23</v>
       </c>
       <c r="O18" s="30" t="s">
+        <v>120</v>
+      </c>
+      <c r="P18" s="31" t="s">
         <v>121</v>
-      </c>
-      <c r="P18" s="31" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4578,10 +4842,10 @@
         <v>73</v>
       </c>
       <c r="B19" s="22" t="s">
+        <v>122</v>
+      </c>
+      <c r="C19" s="23" t="s">
         <v>123</v>
-      </c>
-      <c r="C19" s="23" t="s">
-        <v>124</v>
       </c>
       <c r="D19" s="24" t="n">
         <v>14.016</v>
@@ -4606,22 +4870,22 @@
         <v>19</v>
       </c>
       <c r="K19" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="L19" s="28" t="s">
         <v>125</v>
       </c>
-      <c r="L19" s="28" t="s">
+      <c r="M19" s="28" t="s">
         <v>126</v>
-      </c>
-      <c r="M19" s="28" t="s">
-        <v>127</v>
       </c>
       <c r="N19" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="O19" s="39" t="s">
+      <c r="O19" s="30" t="s">
+        <v>127</v>
+      </c>
+      <c r="P19" s="31" t="s">
         <v>128</v>
-      </c>
-      <c r="P19" s="31" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4629,10 +4893,10 @@
         <v>73</v>
       </c>
       <c r="B20" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="C20" s="23" t="s">
         <v>130</v>
-      </c>
-      <c r="C20" s="23" t="s">
-        <v>131</v>
       </c>
       <c r="D20" s="24" t="n">
         <v>7.3584</v>
@@ -4660,30 +4924,30 @@
         <v>20</v>
       </c>
       <c r="L20" s="28" t="s">
+        <v>131</v>
+      </c>
+      <c r="M20" s="28" t="s">
         <v>132</v>
-      </c>
-      <c r="M20" s="28" t="s">
-        <v>133</v>
       </c>
       <c r="N20" s="29" t="s">
         <v>23</v>
       </c>
       <c r="O20" s="30" t="s">
+        <v>133</v>
+      </c>
+      <c r="P20" s="31" t="s">
         <v>134</v>
-      </c>
-      <c r="P20" s="31" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="22" t="s">
+        <v>135</v>
+      </c>
+      <c r="B21" s="22" t="s">
         <v>136</v>
       </c>
-      <c r="B21" s="22" t="s">
+      <c r="C21" s="23" t="s">
         <v>137</v>
-      </c>
-      <c r="C21" s="23" t="s">
-        <v>138</v>
       </c>
       <c r="D21" s="24" t="n">
         <v>1.752</v>
@@ -4711,7 +4975,7 @@
         <v>8760</v>
       </c>
       <c r="L21" s="28" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="M21" s="27" t="n">
         <v>9.54</v>
@@ -4720,21 +4984,21 @@
         <v>0.00624</v>
       </c>
       <c r="O21" s="30" t="s">
+        <v>139</v>
+      </c>
+      <c r="P21" s="31" t="s">
         <v>140</v>
-      </c>
-      <c r="P21" s="31" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="22" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B22" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="C22" s="23" t="s">
         <v>142</v>
-      </c>
-      <c r="C22" s="23" t="s">
-        <v>143</v>
       </c>
       <c r="D22" s="24" t="n">
         <v>0</v>
@@ -4772,18 +5036,18 @@
       </c>
       <c r="O22" s="30"/>
       <c r="P22" s="31" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="22" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B23" s="22" t="s">
+        <v>144</v>
+      </c>
+      <c r="C23" s="23" t="s">
         <v>145</v>
-      </c>
-      <c r="C23" s="23" t="s">
-        <v>146</v>
       </c>
       <c r="D23" s="24" t="n">
         <v>0.028032</v>
@@ -4795,8 +5059,8 @@
       <c r="F23" s="25" t="n">
         <v>0.20949904</v>
       </c>
-      <c r="G23" s="40" t="s">
-        <v>147</v>
+      <c r="G23" s="38" t="s">
+        <v>146</v>
       </c>
       <c r="H23" s="26" t="n">
         <v>15</v>
@@ -4811,7 +5075,7 @@
         <v>8760</v>
       </c>
       <c r="L23" s="28" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="M23" s="32" t="n">
         <v>0.20939904</v>
@@ -4820,22 +5084,22 @@
         <v>23</v>
       </c>
       <c r="O23" s="30" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="P23" s="31"/>
     </row>
     <row r="24" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="B24" s="22" t="s">
         <v>150</v>
       </c>
-      <c r="B24" s="22" t="s">
+      <c r="C24" s="23" t="s">
         <v>151</v>
       </c>
-      <c r="C24" s="23" t="s">
+      <c r="D24" s="39" t="s">
         <v>152</v>
-      </c>
-      <c r="D24" s="41" t="s">
-        <v>153</v>
       </c>
       <c r="E24" s="25" t="n">
         <f aca="false">F24/H24</f>
@@ -4851,13 +5115,13 @@
         <v>15</v>
       </c>
       <c r="I24" s="28" t="s">
+        <v>153</v>
+      </c>
+      <c r="J24" s="29" t="s">
+        <v>152</v>
+      </c>
+      <c r="K24" s="28" t="s">
         <v>154</v>
-      </c>
-      <c r="J24" s="29" t="s">
-        <v>153</v>
-      </c>
-      <c r="K24" s="28" t="s">
-        <v>155</v>
       </c>
       <c r="L24" s="32" t="n">
         <v>304.67</v>
@@ -4869,21 +5133,21 @@
         <v>23</v>
       </c>
       <c r="O24" s="30" t="s">
+        <v>155</v>
+      </c>
+      <c r="P24" s="31" t="s">
         <v>156</v>
-      </c>
-      <c r="P24" s="31" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="22" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B25" s="22" t="s">
+        <v>157</v>
+      </c>
+      <c r="C25" s="23" t="s">
         <v>158</v>
-      </c>
-      <c r="C25" s="23" t="s">
-        <v>159</v>
       </c>
       <c r="D25" s="24" t="n">
         <v>26.28</v>
@@ -4911,7 +5175,7 @@
         <v>8760</v>
       </c>
       <c r="L25" s="28" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="M25" s="32" t="n">
         <v>598</v>
@@ -4920,21 +5184,21 @@
         <v>0.179</v>
       </c>
       <c r="O25" s="30" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="P25" s="31" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="22" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B26" s="22" t="s">
+        <v>161</v>
+      </c>
+      <c r="C26" s="23" t="s">
         <v>162</v>
-      </c>
-      <c r="C26" s="23" t="s">
-        <v>163</v>
       </c>
       <c r="D26" s="24" t="n">
         <v>8.99998</v>
@@ -4962,33 +5226,33 @@
         <v>19</v>
       </c>
       <c r="L26" s="28" t="s">
+        <v>163</v>
+      </c>
+      <c r="M26" s="33" t="s">
         <v>164</v>
-      </c>
-      <c r="M26" s="33" t="s">
-        <v>165</v>
       </c>
       <c r="N26" s="29" t="s">
         <v>23</v>
       </c>
       <c r="O26" s="30" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="P26" s="31" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="22" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B27" s="22" t="s">
+        <v>166</v>
+      </c>
+      <c r="C27" s="23" t="s">
         <v>167</v>
       </c>
-      <c r="C27" s="23" t="s">
+      <c r="D27" s="40" t="s">
         <v>168</v>
-      </c>
-      <c r="D27" s="42" t="s">
-        <v>169</v>
       </c>
       <c r="E27" s="25" t="n">
         <f aca="false">F27/H27</f>
@@ -5013,32 +5277,32 @@
         <v>19</v>
       </c>
       <c r="L27" s="28" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="M27" s="33" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="N27" s="29" t="s">
         <v>23</v>
       </c>
       <c r="O27" s="30" t="s">
+        <v>170</v>
+      </c>
+      <c r="P27" s="31" t="s">
         <v>171</v>
-      </c>
-      <c r="P27" s="31" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="22" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B28" s="22" t="s">
+        <v>172</v>
+      </c>
+      <c r="C28" s="23" t="s">
         <v>173</v>
       </c>
-      <c r="C28" s="23" t="s">
-        <v>174</v>
-      </c>
-      <c r="D28" s="41" t="n">
+      <c r="D28" s="39" t="n">
         <v>14.892</v>
       </c>
       <c r="E28" s="25" t="n">
@@ -5064,32 +5328,32 @@
         <v>8760</v>
       </c>
       <c r="L28" s="28" t="s">
+        <v>174</v>
+      </c>
+      <c r="M28" s="28" t="s">
         <v>175</v>
-      </c>
-      <c r="M28" s="28" t="s">
-        <v>176</v>
       </c>
       <c r="N28" s="29" t="s">
         <v>23</v>
       </c>
       <c r="O28" s="30" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="P28" s="31" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="22" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B29" s="22" t="s">
+        <v>177</v>
+      </c>
+      <c r="C29" s="23" t="s">
         <v>178</v>
       </c>
-      <c r="C29" s="23" t="s">
-        <v>179</v>
-      </c>
-      <c r="D29" s="41" t="n">
+      <c r="D29" s="39" t="n">
         <v>11</v>
       </c>
       <c r="E29" s="25" t="n">
@@ -5115,32 +5379,32 @@
         <v>8760</v>
       </c>
       <c r="L29" s="28" t="s">
+        <v>179</v>
+      </c>
+      <c r="M29" s="28" t="s">
         <v>180</v>
-      </c>
-      <c r="M29" s="28" t="s">
-        <v>181</v>
       </c>
       <c r="N29" s="29" t="s">
         <v>23</v>
       </c>
       <c r="O29" s="30" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="P29" s="31" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="22" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B30" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="C30" s="23" t="s">
         <v>183</v>
       </c>
-      <c r="C30" s="23" t="s">
-        <v>184</v>
-      </c>
-      <c r="D30" s="41" t="n">
+      <c r="D30" s="39" t="n">
         <v>18</v>
       </c>
       <c r="E30" s="25" t="n">
@@ -5166,32 +5430,32 @@
         <v>8760</v>
       </c>
       <c r="L30" s="28" t="s">
+        <v>184</v>
+      </c>
+      <c r="M30" s="28" t="s">
         <v>185</v>
-      </c>
-      <c r="M30" s="28" t="s">
-        <v>186</v>
       </c>
       <c r="N30" s="29" t="s">
         <v>23</v>
       </c>
       <c r="O30" s="30" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="P30" s="31" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="22" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B31" s="22" t="s">
+        <v>187</v>
+      </c>
+      <c r="C31" s="23" t="s">
         <v>188</v>
       </c>
-      <c r="C31" s="23" t="s">
-        <v>189</v>
-      </c>
-      <c r="D31" s="41" t="n">
+      <c r="D31" s="39" t="n">
         <v>4</v>
       </c>
       <c r="E31" s="25" t="n">
@@ -5217,32 +5481,32 @@
         <v>8760</v>
       </c>
       <c r="L31" s="28" t="s">
+        <v>189</v>
+      </c>
+      <c r="M31" s="28" t="s">
         <v>190</v>
-      </c>
-      <c r="M31" s="28" t="s">
-        <v>191</v>
       </c>
       <c r="N31" s="29" t="s">
         <v>23</v>
       </c>
       <c r="O31" s="30" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="P31" s="31" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="22" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B32" s="22" t="s">
+        <v>192</v>
+      </c>
+      <c r="C32" s="23" t="s">
         <v>193</v>
       </c>
-      <c r="C32" s="23" t="s">
-        <v>194</v>
-      </c>
-      <c r="D32" s="41" t="n">
+      <c r="D32" s="39" t="n">
         <v>3.066</v>
       </c>
       <c r="E32" s="25" t="n">
@@ -5268,32 +5532,32 @@
         <v>8760</v>
       </c>
       <c r="L32" s="28" t="s">
+        <v>194</v>
+      </c>
+      <c r="M32" s="28" t="s">
         <v>195</v>
-      </c>
-      <c r="M32" s="28" t="s">
-        <v>196</v>
       </c>
       <c r="N32" s="29" t="s">
         <v>23</v>
       </c>
       <c r="O32" s="30" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="P32" s="31" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="22" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B33" s="22" t="s">
+        <v>197</v>
+      </c>
+      <c r="C33" s="23" t="s">
         <v>198</v>
       </c>
-      <c r="C33" s="23" t="s">
-        <v>199</v>
-      </c>
-      <c r="D33" s="41" t="n">
+      <c r="D33" s="39" t="n">
         <v>70.08</v>
       </c>
       <c r="E33" s="25" t="n">
@@ -5319,32 +5583,32 @@
         <v>8760</v>
       </c>
       <c r="L33" s="27" t="s">
+        <v>199</v>
+      </c>
+      <c r="M33" s="28" t="s">
         <v>200</v>
-      </c>
-      <c r="M33" s="28" t="s">
-        <v>201</v>
       </c>
       <c r="N33" s="29" t="s">
         <v>23</v>
       </c>
       <c r="O33" s="30" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="P33" s="31" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="22" t="s">
+        <v>202</v>
+      </c>
+      <c r="B34" s="22" t="s">
         <v>203</v>
       </c>
-      <c r="B34" s="22" t="s">
+      <c r="C34" s="23" t="s">
         <v>204</v>
       </c>
-      <c r="C34" s="23" t="s">
-        <v>205</v>
-      </c>
-      <c r="D34" s="41" t="n">
+      <c r="D34" s="39" t="n">
         <v>0</v>
       </c>
       <c r="E34" s="25" t="n">
@@ -5380,20 +5644,20 @@
       </c>
       <c r="O34" s="30"/>
       <c r="P34" s="31" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="22" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B35" s="22" t="s">
+        <v>206</v>
+      </c>
+      <c r="C35" s="23" t="s">
         <v>207</v>
       </c>
-      <c r="C35" s="23" t="s">
-        <v>208</v>
-      </c>
-      <c r="D35" s="41" t="n">
+      <c r="D35" s="39" t="n">
         <v>0</v>
       </c>
       <c r="E35" s="25" t="n">
@@ -5429,20 +5693,20 @@
       </c>
       <c r="O35" s="30"/>
       <c r="P35" s="31" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="22" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B36" s="22" t="s">
+        <v>209</v>
+      </c>
+      <c r="C36" s="23" t="s">
         <v>210</v>
       </c>
-      <c r="C36" s="23" t="s">
-        <v>211</v>
-      </c>
-      <c r="D36" s="41" t="n">
+      <c r="D36" s="39" t="n">
         <v>0</v>
       </c>
       <c r="E36" s="25" t="n">
@@ -5478,20 +5742,20 @@
       </c>
       <c r="O36" s="30"/>
       <c r="P36" s="31" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="22" t="s">
+        <v>212</v>
+      </c>
+      <c r="B37" s="22" t="s">
         <v>213</v>
       </c>
-      <c r="B37" s="22" t="s">
+      <c r="C37" s="23" t="s">
         <v>214</v>
       </c>
-      <c r="C37" s="23" t="s">
-        <v>215</v>
-      </c>
-      <c r="D37" s="41" t="n">
+      <c r="D37" s="39" t="n">
         <v>8.76</v>
       </c>
       <c r="E37" s="25" t="n">
@@ -5514,35 +5778,35 @@
         <v>19</v>
       </c>
       <c r="K37" s="28" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L37" s="28" t="s">
+        <v>215</v>
+      </c>
+      <c r="M37" s="28" t="s">
         <v>216</v>
-      </c>
-      <c r="M37" s="28" t="s">
-        <v>217</v>
       </c>
       <c r="N37" s="29" t="s">
         <v>23</v>
       </c>
       <c r="O37" s="30" t="s">
+        <v>217</v>
+      </c>
+      <c r="P37" s="31" t="s">
         <v>218</v>
-      </c>
-      <c r="P37" s="31" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="22" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B38" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C38" s="23" t="s">
         <v>220</v>
       </c>
-      <c r="C38" s="23" t="s">
-        <v>221</v>
-      </c>
-      <c r="D38" s="41" t="n">
+      <c r="D38" s="39" t="n">
         <v>26.28</v>
       </c>
       <c r="E38" s="25" t="n">
@@ -5559,41 +5823,41 @@
         <v>20</v>
       </c>
       <c r="I38" s="28" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="J38" s="27" t="s">
         <v>19</v>
       </c>
       <c r="K38" s="28" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L38" s="28" t="s">
+        <v>222</v>
+      </c>
+      <c r="M38" s="28" t="s">
         <v>223</v>
-      </c>
-      <c r="M38" s="28" t="s">
-        <v>224</v>
       </c>
       <c r="N38" s="29" t="s">
         <v>23</v>
       </c>
       <c r="O38" s="30" t="s">
+        <v>224</v>
+      </c>
+      <c r="P38" s="31" t="s">
         <v>225</v>
-      </c>
-      <c r="P38" s="31" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="22" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B39" s="22" t="s">
+        <v>226</v>
+      </c>
+      <c r="C39" s="23" t="s">
         <v>227</v>
       </c>
-      <c r="C39" s="23" t="s">
-        <v>228</v>
-      </c>
-      <c r="D39" s="41" t="n">
+      <c r="D39" s="39" t="n">
         <v>210.24</v>
       </c>
       <c r="E39" s="25" t="n">
@@ -5619,32 +5883,32 @@
         <v>8760</v>
       </c>
       <c r="L39" s="28" t="s">
+        <v>228</v>
+      </c>
+      <c r="M39" s="33" t="s">
         <v>229</v>
-      </c>
-      <c r="M39" s="33" t="s">
-        <v>230</v>
       </c>
       <c r="N39" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="O39" s="39" t="s">
+      <c r="O39" s="30" t="s">
+        <v>230</v>
+      </c>
+      <c r="P39" s="31" t="s">
         <v>231</v>
-      </c>
-      <c r="P39" s="31" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="22" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B40" s="22" t="s">
+        <v>232</v>
+      </c>
+      <c r="C40" s="23" t="s">
         <v>233</v>
       </c>
-      <c r="C40" s="23" t="s">
-        <v>234</v>
-      </c>
-      <c r="D40" s="41" t="n">
+      <c r="D40" s="39" t="n">
         <v>87.6</v>
       </c>
       <c r="E40" s="25" t="n">
@@ -5670,32 +5934,32 @@
         <v>8760</v>
       </c>
       <c r="L40" s="28" t="s">
+        <v>234</v>
+      </c>
+      <c r="M40" s="33" t="s">
         <v>235</v>
-      </c>
-      <c r="M40" s="33" t="s">
-        <v>236</v>
       </c>
       <c r="N40" s="29" t="s">
         <v>23</v>
       </c>
       <c r="O40" s="30" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="P40" s="31" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="22" t="s">
+        <v>237</v>
+      </c>
+      <c r="B41" s="22" t="s">
+        <v>238</v>
+      </c>
+      <c r="C41" s="23" t="s">
         <v>239</v>
       </c>
-      <c r="B41" s="22" t="s">
-        <v>240</v>
-      </c>
-      <c r="C41" s="23" t="s">
-        <v>241</v>
-      </c>
-      <c r="D41" s="41" t="n">
+      <c r="D41" s="39" t="n">
         <v>0</v>
       </c>
       <c r="E41" s="25" t="n">
@@ -5731,18 +5995,18 @@
       </c>
       <c r="O41" s="30"/>
       <c r="P41" s="31" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="22" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B42" s="22" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C42" s="23" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D42" s="24" t="n">
         <v>919.8</v>
@@ -5761,39 +6025,39 @@
         <v>6</v>
       </c>
       <c r="I42" s="33" t="s">
+        <v>243</v>
+      </c>
+      <c r="J42" s="41" t="s">
+        <v>19</v>
+      </c>
+      <c r="K42" s="33" t="s">
+        <v>154</v>
+      </c>
+      <c r="L42" s="41" t="n">
+        <v>106.69</v>
+      </c>
+      <c r="M42" s="33" t="s">
+        <v>244</v>
+      </c>
+      <c r="N42" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="O42" s="30" t="s">
         <v>245</v>
       </c>
-      <c r="J42" s="43" t="s">
-        <v>19</v>
-      </c>
-      <c r="K42" s="33" t="s">
-        <v>155</v>
-      </c>
-      <c r="L42" s="43" t="n">
-        <v>106.69</v>
-      </c>
-      <c r="M42" s="33" t="s">
+      <c r="P42" s="31" t="s">
         <v>246</v>
-      </c>
-      <c r="N42" s="44" t="s">
-        <v>23</v>
-      </c>
-      <c r="O42" s="30" t="s">
-        <v>247</v>
-      </c>
-      <c r="P42" s="31" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="22" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B43" s="22" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C43" s="23" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D43" s="24" t="n">
         <v>345.144</v>
@@ -5818,33 +6082,33 @@
         <v>1.9</v>
       </c>
       <c r="K43" s="33" t="s">
-        <v>155</v>
-      </c>
-      <c r="L43" s="43" t="n">
+        <v>154</v>
+      </c>
+      <c r="L43" s="41" t="n">
         <v>222.75</v>
       </c>
       <c r="M43" s="33" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="N43" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="O43" s="45" t="s">
-        <v>252</v>
+      <c r="O43" s="43" t="s">
+        <v>250</v>
       </c>
       <c r="P43" s="31" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="22" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B44" s="22" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C44" s="23" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="D44" s="24" t="n">
         <v>115.632</v>
@@ -5869,135 +6133,135 @@
         <v>1.84</v>
       </c>
       <c r="K44" s="33" t="s">
-        <v>155</v>
-      </c>
-      <c r="L44" s="43" t="n">
+        <v>154</v>
+      </c>
+      <c r="L44" s="41" t="n">
         <v>169.91</v>
       </c>
       <c r="M44" s="33" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="N44" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="O44" s="45" t="s">
-        <v>252</v>
+      <c r="O44" s="43" t="s">
+        <v>250</v>
       </c>
       <c r="P44" s="31" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="44" t="s">
+        <v>237</v>
+      </c>
+      <c r="B45" s="44" t="s">
+        <v>256</v>
+      </c>
+      <c r="C45" s="45" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="45" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="46" t="s">
-        <v>239</v>
-      </c>
-      <c r="B45" s="46" t="s">
-        <v>258</v>
-      </c>
-      <c r="C45" s="47" t="s">
-        <v>259</v>
-      </c>
-      <c r="D45" s="48" t="n">
+      <c r="D45" s="46" t="n">
         <v>94</v>
       </c>
-      <c r="E45" s="49" t="n">
+      <c r="E45" s="47" t="n">
         <f aca="false">F45/H45</f>
         <v>81.457</v>
       </c>
-      <c r="F45" s="49" t="n">
+      <c r="F45" s="47" t="n">
         <v>814.57</v>
       </c>
-      <c r="G45" s="49" t="n">
+      <c r="G45" s="47" t="n">
         <v>2.6</v>
       </c>
-      <c r="H45" s="50" t="n">
+      <c r="H45" s="48" t="n">
         <v>10</v>
       </c>
-      <c r="I45" s="51" t="n">
+      <c r="I45" s="49" t="n">
         <v>47</v>
       </c>
-      <c r="J45" s="52" t="s">
+      <c r="J45" s="50" t="s">
         <v>19</v>
       </c>
-      <c r="K45" s="53" t="s">
+      <c r="K45" s="51" t="s">
+        <v>258</v>
+      </c>
+      <c r="L45" s="51" t="n">
+        <v>346.45</v>
+      </c>
+      <c r="M45" s="51" t="s">
+        <v>259</v>
+      </c>
+      <c r="N45" s="52" t="s">
+        <v>23</v>
+      </c>
+      <c r="O45" s="53" t="s">
         <v>260</v>
       </c>
-      <c r="L45" s="53" t="n">
-        <v>346.45</v>
-      </c>
-      <c r="M45" s="53" t="s">
+      <c r="P45" s="54" t="s">
         <v>261</v>
       </c>
-      <c r="N45" s="54" t="s">
-        <v>23</v>
-      </c>
-      <c r="O45" s="55" t="s">
-        <v>262</v>
-      </c>
-      <c r="P45" s="56" t="s">
-        <v>263</v>
-      </c>
     </row>
     <row r="46" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M46" s="57"/>
-      <c r="O46" s="57"/>
+      <c r="M46" s="55"/>
+      <c r="O46" s="55"/>
     </row>
     <row r="47" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M47" s="57"/>
-      <c r="O47" s="57"/>
+      <c r="M47" s="55"/>
+      <c r="O47" s="55"/>
     </row>
     <row r="48" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I48" s="34"/>
       <c r="J48" s="34"/>
       <c r="K48" s="34"/>
-      <c r="M48" s="57"/>
-      <c r="O48" s="57"/>
+      <c r="M48" s="55"/>
+      <c r="O48" s="55"/>
     </row>
     <row r="49" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I49" s="34"/>
       <c r="J49" s="34"/>
       <c r="K49" s="34"/>
-      <c r="M49" s="57"/>
-      <c r="O49" s="57"/>
+      <c r="M49" s="55"/>
+      <c r="O49" s="55"/>
     </row>
     <row r="50" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M50" s="57"/>
-      <c r="O50" s="57"/>
+      <c r="M50" s="55"/>
+      <c r="O50" s="55"/>
     </row>
     <row r="51" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M51" s="57"/>
-      <c r="N51" s="58"/>
-      <c r="O51" s="57"/>
+      <c r="M51" s="55"/>
+      <c r="N51" s="56"/>
+      <c r="O51" s="55"/>
     </row>
     <row r="52" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M52" s="57"/>
-      <c r="N52" s="58"/>
-      <c r="O52" s="57"/>
+      <c r="M52" s="55"/>
+      <c r="N52" s="56"/>
+      <c r="O52" s="55"/>
     </row>
     <row r="53" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M53" s="57"/>
-      <c r="N53" s="58"/>
-      <c r="O53" s="57"/>
+      <c r="M53" s="55"/>
+      <c r="N53" s="56"/>
+      <c r="O53" s="55"/>
     </row>
     <row r="54" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M54" s="57"/>
-      <c r="O54" s="57"/>
+      <c r="M54" s="55"/>
+      <c r="O54" s="55"/>
     </row>
     <row r="55" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M55" s="57"/>
-      <c r="O55" s="57"/>
+      <c r="M55" s="55"/>
+      <c r="O55" s="55"/>
     </row>
     <row r="56" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M56" s="57"/>
-      <c r="O56" s="57"/>
+      <c r="M56" s="55"/>
+      <c r="O56" s="55"/>
     </row>
     <row r="57" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M57" s="57"/>
-      <c r="O57" s="57"/>
+      <c r="M57" s="55"/>
+      <c r="O57" s="55"/>
     </row>
     <row r="58" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M58" s="57"/>
-      <c r="O58" s="57"/>
+      <c r="M58" s="55"/>
+      <c r="O58" s="55"/>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
@@ -6018,8 +6282,8 @@
   </sheetPr>
   <dimension ref="A1:AF46"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M41" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AB50" activeCellId="0" sqref="AB50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.37109375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6030,13 +6294,13 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="120.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="60" t="s">
+      <c r="B1" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="60" t="s">
+      <c r="C1" s="58" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
@@ -6076,7 +6340,7 @@
         <v>14</v>
       </c>
       <c r="P1" s="7" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="Q1" s="4" t="s">
         <v>3</v>
@@ -6115,7 +6379,7 @@
         <v>14</v>
       </c>
       <c r="AC1" s="7" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="AD1" s="4" t="s">
         <v>3</v>
@@ -6127,629 +6391,646 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="61" t="s">
+    <row r="2" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="59" t="s">
+        <v>263</v>
+      </c>
+      <c r="B2" s="59" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="60" t="s">
+        <v>264</v>
+      </c>
+      <c r="AB2" s="61" t="s">
         <v>265</v>
       </c>
-      <c r="B2" s="61" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="62" t="s">
+    </row>
+    <row r="3" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="59" t="s">
+        <v>263</v>
+      </c>
+      <c r="B3" s="59" t="s">
         <v>266</v>
       </c>
-      <c r="AB2" s="63" t="s">
+      <c r="C3" s="60" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="61" t="s">
-        <v>265</v>
-      </c>
-      <c r="B3" s="61" t="s">
+      <c r="AB3" s="62" t="s">
         <v>268</v>
       </c>
-      <c r="C3" s="62" t="s">
+    </row>
+    <row r="4" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="59" t="s">
+        <v>263</v>
+      </c>
+      <c r="B4" s="59" t="s">
         <v>269</v>
       </c>
-      <c r="AB3" s="61" t="s">
+      <c r="C4" s="60" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="61" t="s">
-        <v>265</v>
-      </c>
-      <c r="B4" s="61" t="s">
+      <c r="AB4" s="62" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="59" t="s">
+        <v>263</v>
+      </c>
+      <c r="B5" s="59" t="s">
         <v>271</v>
       </c>
-      <c r="C4" s="62" t="s">
+      <c r="C5" s="60" t="s">
         <v>272</v>
       </c>
-      <c r="AB4" s="61" t="s">
+      <c r="AB5" s="59" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="61" t="s">
-        <v>265</v>
-      </c>
-      <c r="B5" s="61" t="s">
+    <row r="6" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="59" t="s">
+        <v>263</v>
+      </c>
+      <c r="B6" s="59" t="s">
         <v>274</v>
       </c>
-      <c r="C5" s="62" t="s">
+      <c r="C6" s="60" t="s">
         <v>275</v>
       </c>
-      <c r="AB5" s="61" t="s">
+      <c r="AB6" s="59" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="61" t="s">
-        <v>265</v>
-      </c>
-      <c r="B6" s="61" t="s">
+    <row r="7" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="59" t="s">
+        <v>263</v>
+      </c>
+      <c r="B7" s="59" t="s">
         <v>277</v>
       </c>
-      <c r="C6" s="62" t="s">
+      <c r="C7" s="60" t="s">
         <v>278</v>
       </c>
-      <c r="AB6" s="61" t="s">
+      <c r="AB7" s="59" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="61" t="s">
-        <v>265</v>
-      </c>
-      <c r="B7" s="61" t="s">
+    <row r="8" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="59" t="s">
+        <v>263</v>
+      </c>
+      <c r="B8" s="59" t="s">
         <v>280</v>
       </c>
-      <c r="C7" s="62" t="s">
+      <c r="C8" s="60" t="s">
         <v>281</v>
       </c>
-      <c r="AB7" s="61" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="61" t="s">
-        <v>265</v>
-      </c>
-      <c r="B8" s="61" t="s">
+      <c r="AB8" s="59" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="59" t="s">
+        <v>263</v>
+      </c>
+      <c r="B9" s="59" t="s">
         <v>282</v>
       </c>
-      <c r="C8" s="62" t="s">
+      <c r="C9" s="60" t="s">
         <v>283</v>
       </c>
-      <c r="AB8" s="61" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="61" t="s">
-        <v>265</v>
-      </c>
-      <c r="B9" s="61" t="s">
+      <c r="AB9" s="59" t="s">
         <v>284</v>
       </c>
-      <c r="C9" s="62" t="s">
+    </row>
+    <row r="10" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="59" t="s">
+        <v>263</v>
+      </c>
+      <c r="B10" s="59" t="s">
         <v>285</v>
       </c>
-      <c r="AB9" s="61" t="s">
+      <c r="C10" s="60" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="61" t="s">
-        <v>265</v>
-      </c>
-      <c r="B10" s="61" t="s">
+      <c r="AB10" s="61" t="s">
         <v>287</v>
       </c>
-      <c r="C10" s="62" t="s">
+    </row>
+    <row r="11" customFormat="false" ht="180.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="59" t="s">
         <v>288</v>
       </c>
-      <c r="AB10" s="63" t="s">
+      <c r="B11" s="59" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="61" t="s">
+      <c r="C11" s="60" t="s">
         <v>290</v>
       </c>
-      <c r="B11" s="61" t="s">
+      <c r="AB11" s="59" t="s">
         <v>291</v>
       </c>
-      <c r="C11" s="62" t="s">
+    </row>
+    <row r="12" customFormat="false" ht="180.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="59" t="s">
+        <v>288</v>
+      </c>
+      <c r="B12" s="59" t="s">
         <v>292</v>
       </c>
-      <c r="AB11" s="61" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="61" t="s">
-        <v>290</v>
-      </c>
-      <c r="B12" s="61" t="s">
+      <c r="C12" s="60" t="s">
         <v>293</v>
       </c>
-      <c r="C12" s="62" t="s">
+      <c r="AB12" s="59" t="s">
         <v>294</v>
       </c>
-      <c r="AB12" s="61" t="s">
+    </row>
+    <row r="13" customFormat="false" ht="180.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="59" t="s">
+        <v>288</v>
+      </c>
+      <c r="B13" s="59" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="13" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="61" t="s">
-        <v>290</v>
-      </c>
-      <c r="B13" s="61" t="s">
+      <c r="C13" s="60" t="s">
         <v>296</v>
       </c>
-      <c r="C13" s="62" t="s">
+      <c r="AB13" s="59" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="59" t="s">
+        <v>288</v>
+      </c>
+      <c r="B14" s="59" t="s">
         <v>297</v>
       </c>
-      <c r="AB13" s="61" t="s">
+      <c r="C14" s="60" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="14" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="61" t="s">
-        <v>290</v>
-      </c>
-      <c r="B14" s="61" t="s">
+      <c r="AB14" s="59" t="s">
         <v>299</v>
       </c>
-      <c r="C14" s="62" t="s">
+    </row>
+    <row r="15" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="59" t="s">
+        <v>288</v>
+      </c>
+      <c r="B15" s="59" t="s">
         <v>300</v>
       </c>
-      <c r="AB14" s="61" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="61" t="s">
-        <v>290</v>
-      </c>
-      <c r="B15" s="61" t="s">
+      <c r="C15" s="60" t="s">
         <v>301</v>
       </c>
-      <c r="C15" s="62" t="s">
+      <c r="AB15" s="59" t="s">
         <v>302</v>
       </c>
-      <c r="AB15" s="61" t="s">
+    </row>
+    <row r="16" customFormat="false" ht="191.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="59" t="s">
+        <v>288</v>
+      </c>
+      <c r="B16" s="59" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="16" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="61" t="s">
-        <v>290</v>
-      </c>
-      <c r="B16" s="61" t="s">
+      <c r="C16" s="60" t="s">
         <v>304</v>
       </c>
-      <c r="C16" s="62" t="s">
+      <c r="AB16" s="59" t="s">
         <v>305</v>
       </c>
-      <c r="AB16" s="61" t="s">
+    </row>
+    <row r="17" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="59" t="s">
+        <v>288</v>
+      </c>
+      <c r="B17" s="59" t="s">
         <v>306</v>
       </c>
-    </row>
-    <row r="17" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="61" t="s">
-        <v>290</v>
-      </c>
-      <c r="B17" s="61" t="s">
+      <c r="C17" s="60" t="s">
         <v>307</v>
       </c>
-      <c r="C17" s="62" t="s">
+      <c r="AB17" s="59" t="s">
         <v>308</v>
       </c>
-      <c r="AB17" s="61" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="61" t="s">
-        <v>290</v>
-      </c>
-      <c r="B18" s="61" t="s">
+    </row>
+    <row r="18" customFormat="false" ht="180.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="59" t="s">
+        <v>288</v>
+      </c>
+      <c r="B18" s="59" t="s">
         <v>309</v>
       </c>
-      <c r="C18" s="62" t="s">
+      <c r="C18" s="60" t="s">
         <v>310</v>
       </c>
-      <c r="AB18" s="63" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="61" t="s">
-        <v>290</v>
-      </c>
-      <c r="B19" s="61" t="s">
+      <c r="AB18" s="61" t="s">
         <v>311</v>
       </c>
-      <c r="C19" s="62" t="s">
+    </row>
+    <row r="19" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="59" t="s">
+        <v>288</v>
+      </c>
+      <c r="B19" s="59" t="s">
         <v>312</v>
       </c>
-      <c r="AB19" s="61" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="61" t="s">
-        <v>290</v>
-      </c>
-      <c r="B20" s="61" t="s">
+      <c r="C19" s="60" t="s">
         <v>313</v>
       </c>
-      <c r="C20" s="62" t="s">
+      <c r="AB19" s="59" t="s">
         <v>314</v>
       </c>
-      <c r="AB20" s="61" t="s">
-        <v>286</v>
+    </row>
+    <row r="20" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="59" t="s">
+        <v>288</v>
+      </c>
+      <c r="B20" s="59" t="s">
+        <v>315</v>
+      </c>
+      <c r="C20" s="60" t="s">
+        <v>316</v>
+      </c>
+      <c r="AB20" s="59" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="61" t="s">
-        <v>315</v>
-      </c>
-      <c r="B21" s="61" t="s">
-        <v>316</v>
-      </c>
-      <c r="C21" s="62" t="s">
-        <v>317</v>
-      </c>
-      <c r="AB21" s="61" t="s">
+      <c r="A21" s="59" t="s">
         <v>318</v>
       </c>
+      <c r="B21" s="59" t="s">
+        <v>319</v>
+      </c>
+      <c r="C21" s="60" t="s">
+        <v>320</v>
+      </c>
+      <c r="AB21" s="62" t="s">
+        <v>321</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="61" t="s">
-        <v>315</v>
-      </c>
-      <c r="B22" s="61" t="s">
-        <v>319</v>
-      </c>
-      <c r="C22" s="62" t="s">
-        <v>320</v>
-      </c>
-      <c r="AB22" s="61" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="61" t="s">
-        <v>315</v>
-      </c>
-      <c r="B23" s="61" t="s">
+      <c r="A22" s="59" t="s">
+        <v>318</v>
+      </c>
+      <c r="B22" s="59" t="s">
+        <v>322</v>
+      </c>
+      <c r="C22" s="60" t="s">
+        <v>323</v>
+      </c>
+      <c r="AB22" s="59" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="59" t="s">
+        <v>318</v>
+      </c>
+      <c r="B23" s="59" t="s">
+        <v>325</v>
+      </c>
+      <c r="C23" s="60" t="s">
+        <v>326</v>
+      </c>
+      <c r="AB23" s="63" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="59" t="s">
+        <v>318</v>
+      </c>
+      <c r="B24" s="59" t="s">
+        <v>328</v>
+      </c>
+      <c r="C24" s="60" t="s">
+        <v>329</v>
+      </c>
+      <c r="AB24" s="59" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="59" t="s">
+        <v>318</v>
+      </c>
+      <c r="B25" s="59" t="s">
+        <v>331</v>
+      </c>
+      <c r="C25" s="60" t="s">
+        <v>332</v>
+      </c>
+      <c r="AB25" s="63" t="s">
         <v>321</v>
       </c>
-      <c r="C23" s="62" t="s">
-        <v>322</v>
-      </c>
-      <c r="AB23" s="63" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="61" t="s">
-        <v>315</v>
-      </c>
-      <c r="B24" s="61" t="s">
-        <v>324</v>
-      </c>
-      <c r="C24" s="62" t="s">
-        <v>325</v>
-      </c>
-      <c r="AB24" s="61" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="61" t="s">
-        <v>315</v>
-      </c>
-      <c r="B25" s="61" t="s">
-        <v>327</v>
-      </c>
-      <c r="C25" s="62" t="s">
-        <v>328</v>
-      </c>
-      <c r="AB25" s="63" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="61" t="s">
-        <v>315</v>
-      </c>
-      <c r="B26" s="61" t="s">
-        <v>330</v>
-      </c>
-      <c r="C26" s="62" t="s">
-        <v>331</v>
-      </c>
-      <c r="AB26" s="61" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="61" t="s">
-        <v>315</v>
-      </c>
-      <c r="B27" s="61" t="s">
+    </row>
+    <row r="26" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="59" t="s">
+        <v>318</v>
+      </c>
+      <c r="B26" s="59" t="s">
         <v>333</v>
       </c>
-      <c r="C27" s="62" t="s">
+      <c r="C26" s="60" t="s">
         <v>334</v>
       </c>
-      <c r="AB27" s="61" t="s">
+      <c r="AB26" s="59" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="180.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="59" t="s">
+        <v>318</v>
+      </c>
+      <c r="B27" s="59" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="28" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="61" t="s">
-        <v>315</v>
-      </c>
-      <c r="B28" s="61" t="s">
+      <c r="C27" s="60" t="s">
         <v>336</v>
       </c>
-      <c r="C28" s="62" t="s">
+      <c r="AB27" s="59" t="s">
         <v>337</v>
       </c>
-      <c r="AB28" s="63" t="s">
+    </row>
+    <row r="28" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="59" t="s">
+        <v>318</v>
+      </c>
+      <c r="B28" s="59" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="29" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="61" t="s">
-        <v>315</v>
-      </c>
-      <c r="B29" s="61" t="s">
+      <c r="C28" s="60" t="s">
         <v>339</v>
       </c>
-      <c r="C29" s="62" t="s">
+      <c r="AB28" s="61" t="s">
         <v>340</v>
       </c>
-      <c r="AB29" s="61" t="s">
+    </row>
+    <row r="29" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="59" t="s">
+        <v>318</v>
+      </c>
+      <c r="B29" s="59" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="30" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="61" t="s">
-        <v>315</v>
-      </c>
-      <c r="B30" s="61" t="s">
+      <c r="C29" s="60" t="s">
         <v>342</v>
       </c>
-      <c r="C30" s="62" t="s">
+      <c r="AB29" s="59" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="59" t="s">
+        <v>318</v>
+      </c>
+      <c r="B30" s="59" t="s">
         <v>343</v>
       </c>
-      <c r="AB30" s="61" t="s">
+      <c r="C30" s="60" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="31" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="61" t="s">
-        <v>315</v>
-      </c>
-      <c r="B31" s="61" t="s">
+      <c r="AB30" s="59" t="s">
         <v>345</v>
       </c>
-      <c r="C31" s="62" t="s">
+    </row>
+    <row r="31" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="59" t="s">
+        <v>318</v>
+      </c>
+      <c r="B31" s="59" t="s">
         <v>346</v>
       </c>
-      <c r="AB31" s="61" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="61" t="s">
-        <v>315</v>
-      </c>
-      <c r="B32" s="61" t="s">
+      <c r="C31" s="60" t="s">
         <v>347</v>
       </c>
-      <c r="C32" s="62" t="s">
+      <c r="AB31" s="59" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="59" t="s">
+        <v>318</v>
+      </c>
+      <c r="B32" s="59" t="s">
         <v>348</v>
       </c>
-      <c r="AB32" s="61" t="s">
+      <c r="C32" s="60" t="s">
         <v>349</v>
       </c>
-    </row>
-    <row r="33" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="61" t="s">
-        <v>315</v>
-      </c>
-      <c r="B33" s="61" t="s">
+      <c r="AB32" s="59" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="59" t="s">
+        <v>318</v>
+      </c>
+      <c r="B33" s="59" t="s">
         <v>350</v>
       </c>
-      <c r="C33" s="62" t="s">
+      <c r="C33" s="60" t="s">
         <v>351</v>
       </c>
-      <c r="AB33" s="61" t="s">
+      <c r="AB33" s="59" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="59" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="34" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="61" t="s">
+      <c r="B34" s="59" t="s">
         <v>353</v>
       </c>
-      <c r="B34" s="61" t="s">
+      <c r="C34" s="60" t="s">
         <v>354</v>
       </c>
-      <c r="C34" s="62" t="s">
+      <c r="AB34" s="59"/>
+    </row>
+    <row r="35" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="59" t="s">
+        <v>352</v>
+      </c>
+      <c r="B35" s="59" t="s">
         <v>355</v>
       </c>
-      <c r="AB34" s="61" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="61" t="s">
-        <v>353</v>
-      </c>
-      <c r="B35" s="61" t="s">
+      <c r="C35" s="60" t="s">
         <v>356</v>
       </c>
-      <c r="C35" s="62" t="s">
+    </row>
+    <row r="36" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="59" t="s">
+        <v>352</v>
+      </c>
+      <c r="B36" s="59" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="36" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="61" t="s">
-        <v>353</v>
-      </c>
-      <c r="B36" s="61" t="s">
+      <c r="C36" s="60" t="s">
         <v>358</v>
       </c>
-      <c r="C36" s="62" t="s">
+    </row>
+    <row r="37" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="59" t="s">
+        <v>352</v>
+      </c>
+      <c r="B37" s="59" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="37" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="61" t="s">
-        <v>353</v>
-      </c>
-      <c r="B37" s="61" t="s">
+      <c r="C37" s="60" t="s">
         <v>360</v>
       </c>
-      <c r="C37" s="62" t="s">
+      <c r="AB37" s="59" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="61" t="s">
-        <v>353</v>
-      </c>
-      <c r="B38" s="61" t="s">
-        <v>220</v>
-      </c>
-      <c r="C38" s="62" t="s">
+    <row r="38" customFormat="false" ht="214.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="59" t="s">
+        <v>352</v>
+      </c>
+      <c r="B38" s="59" t="s">
+        <v>219</v>
+      </c>
+      <c r="C38" s="60" t="s">
         <v>362</v>
       </c>
-      <c r="AB38" s="63" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="61" t="s">
-        <v>353</v>
-      </c>
-      <c r="B39" s="61" t="s">
+      <c r="AB38" s="61" t="s">
         <v>363</v>
       </c>
-      <c r="C39" s="62" t="s">
+    </row>
+    <row r="39" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="59" t="s">
+        <v>352</v>
+      </c>
+      <c r="B39" s="59" t="s">
         <v>364</v>
       </c>
-      <c r="AB39" s="61" t="s">
+      <c r="C39" s="60" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="40" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="61" t="s">
-        <v>353</v>
-      </c>
-      <c r="B40" s="61" t="s">
+      <c r="AB39" s="59" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="59" t="s">
+        <v>352</v>
+      </c>
+      <c r="B40" s="59" t="s">
         <v>366</v>
       </c>
-      <c r="C40" s="62" t="s">
+      <c r="C40" s="60" t="s">
         <v>367</v>
       </c>
-      <c r="AB40" s="61" t="s">
+      <c r="AB40" s="59" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="59" t="s">
+        <v>237</v>
+      </c>
+      <c r="B41" s="59" t="s">
         <v>368</v>
       </c>
-    </row>
-    <row r="41" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="61" t="s">
-        <v>239</v>
-      </c>
-      <c r="B41" s="61" t="s">
+      <c r="C41" s="60" t="s">
         <v>369</v>
       </c>
-      <c r="C41" s="62" t="s">
+      <c r="AB41" s="61" t="s">
         <v>370</v>
       </c>
-      <c r="AB41" s="63" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="61" t="s">
-        <v>239</v>
-      </c>
-      <c r="B42" s="61" t="s">
-        <v>243</v>
-      </c>
-      <c r="C42" s="62" t="s">
+    </row>
+    <row r="42" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="59" t="s">
+        <v>237</v>
+      </c>
+      <c r="B42" s="59" t="s">
+        <v>241</v>
+      </c>
+      <c r="C42" s="60" t="s">
         <v>371</v>
       </c>
-      <c r="AB42" s="61" t="s">
+      <c r="AB42" s="59" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="61" t="s">
-        <v>239</v>
-      </c>
-      <c r="B43" s="61" t="s">
-        <v>249</v>
-      </c>
-      <c r="C43" s="62" t="s">
+    <row r="43" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="59" t="s">
+        <v>237</v>
+      </c>
+      <c r="B43" s="59" t="s">
+        <v>247</v>
+      </c>
+      <c r="C43" s="60" t="s">
         <v>373</v>
       </c>
-      <c r="AB43" s="61" t="s">
+      <c r="AB43" s="59" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="61" t="s">
-        <v>239</v>
-      </c>
-      <c r="B44" s="61" t="s">
-        <v>254</v>
-      </c>
-      <c r="C44" s="62" t="s">
+    <row r="44" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="59" t="s">
+        <v>237</v>
+      </c>
+      <c r="B44" s="59" t="s">
+        <v>252</v>
+      </c>
+      <c r="C44" s="60" t="s">
         <v>375</v>
       </c>
-      <c r="AB44" s="61" t="s">
+      <c r="AB44" s="59" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="59" t="s">
+        <v>237</v>
+      </c>
+      <c r="B45" s="59" t="s">
+        <v>256</v>
+      </c>
+      <c r="C45" s="60" t="s">
         <v>376</v>
       </c>
-    </row>
-    <row r="45" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="61" t="s">
-        <v>239</v>
-      </c>
-      <c r="B45" s="61" t="s">
-        <v>258</v>
-      </c>
-      <c r="C45" s="62" t="s">
+      <c r="AB45" s="59" t="s">
         <v>377</v>
       </c>
-      <c r="AB45" s="61" t="s">
-        <v>378</v>
-      </c>
     </row>
     <row r="46" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AB46" s="63" t="s">
-        <v>379</v>
-      </c>
+      <c r="AB46" s="61"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="AB2" r:id="rId1" location="Kraftwerke" display="&lt;sup&gt;a&lt;/sup&gt; Product packaging is included; for the THP, only the mass balance was used, and production processes along with their energy consumption were not considered due to a lack of data; The calculation was performed using the CML-IA Baseline 3.08 method.&#10;&lt;sup&gt;b&lt;/sup&gt; The greenhouse gas potential during the usage phase was calculated based on emission factors for the German electricity mix from the Federal Environment Agency for the year 2022 (https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke);&#10;&lt;sup&gt;c&lt;/sup&gt; Assumed operating time: 24h/day"/>
-    <hyperlink ref="AB10" r:id="rId2" location="Kraftwerke" display="&lt;sup&gt;b&lt;/sup&gt; Greenhouse gas potential during the usage phase was calculated based on emission factors for the German electricity mix provided by the Federal Environment Agency for the year 2022 (https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke);"/>
-    <hyperlink ref="AB18" r:id="rId3" location="Kraftwerke" display="&lt;sup&gt;b&lt;/sup&gt; Greenhouse gas potential during the usage phase was calculated based on emission factors for the German electricity mix provided by the Federal Environment Agency for the year 2022 (https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke);"/>
-    <hyperlink ref="AB23" r:id="rId4" display="&lt;sup&gt;a&lt;/sup&gt; Fan for commercial and light industrial applications, performance calculation by interpolation of values from: https://www.dasslerventilatoren.info/contents/de/d135_WandventilatorECMotor.html, depending on the application, higher performances are also possible."/>
-    <hyperlink ref="AB25" r:id="rId5" location="Kraftwerke" display="&lt;sup&gt;c&lt;/sup&gt; Greenhouse gas potential during the usage phase was calculated based on emission factors for the German electricity mix provided by the Federal Environment Agency for the year 2022 (https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke); Assumed operating time: 10 hours per day."/>
-    <hyperlink ref="AB28" r:id="rId6" location="Kraftwerke" display="&lt;sup&gt;a&lt;/sup&gt; Greenhouse gas potential during the usage phase was calculated based on emission factors for the German electricity mix provided by the Federal Environment Agency for the year 2022 (https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke);"/>
-    <hyperlink ref="AB38" r:id="rId7" location="Kraftwerke" display="&lt;sup&gt;b&lt;/sup&gt; Greenhouse gas potential during the usage phase was calculated based on emission factors for the German electricity mix provided by the Federal Environment Agency for the year 2022 (https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke);"/>
-    <hyperlink ref="AB41" r:id="rId8" location="Kraftwerke" display="&lt;sup&gt;b&lt;/sup&gt; Greenhouse gas potential during the usage phase was calculated based on emission factors for the German electricity mix provided by the Federal Environment Agency for the year 2022 (https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke);"/>
-    <hyperlink ref="AB46" r:id="rId9" location="Kraftwerke" display="&lt;sup&gt;c&lt;/sup&gt; Greenhouse gas potential during the usage phase was calculated based on emission factors for the German electricity mix provided by the Federal Environment Agency for the year 2022 (https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke)."/>
+    <hyperlink ref="AB2" r:id="rId1" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
+    <hyperlink ref="AB5" r:id="rId2" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
+    <hyperlink ref="AB8" r:id="rId3" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
+    <hyperlink ref="AB9" r:id="rId4" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
+    <hyperlink ref="AB15" r:id="rId5" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
+    <hyperlink ref="AB16" r:id="rId6" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
+    <hyperlink ref="AB17" r:id="rId7" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
+    <hyperlink ref="AB18" r:id="rId8" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
+    <hyperlink ref="AB19" r:id="rId9" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
+    <hyperlink ref="AB20" r:id="rId10" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
+    <hyperlink ref="AB26" r:id="rId11" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
+    <hyperlink ref="AB27" r:id="rId12" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
+    <hyperlink ref="AB28" r:id="rId13" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
+    <hyperlink ref="AB29" r:id="rId14" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
+    <hyperlink ref="AB30" r:id="rId15" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
+    <hyperlink ref="AB31" r:id="rId16" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
+    <hyperlink ref="AB32" r:id="rId17" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
+    <hyperlink ref="AB33" r:id="rId18" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
+    <hyperlink ref="AB37" r:id="rId19" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
+    <hyperlink ref="AB38" r:id="rId20" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
+    <hyperlink ref="AB39" r:id="rId21" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
+    <hyperlink ref="AB40" r:id="rId22" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
+    <hyperlink ref="AB41" r:id="rId23" location="Kraftwerke" display="&lt;sup&gt;b&lt;/sup&gt; Greenhouse gas potential during the usage phase was calculated based on emission factors for the German electricity mix provided by the Federal Environment Agency for the year 2022 (https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke);"/>
+    <hyperlink ref="AB42" r:id="rId24" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
+    <hyperlink ref="AB43" r:id="rId25" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
+    <hyperlink ref="AB44" r:id="rId26" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
+    <hyperlink ref="AB45" r:id="rId27" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
changed styling of listing-row, so that superscript elements are shown in its own line
</commit_message>
<xml_diff>
--- a/02_work_doc/01_daten/12_component_list/componentList_oneSheet.xlsx
+++ b/02_work_doc/01_daten/12_component_list/componentList_oneSheet.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="378">
   <si>
     <t xml:space="preserve">Kategorie</t>
   </si>
@@ -3891,8 +3891,8 @@
   </sheetPr>
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="N36" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O45" activeCellId="0" sqref="O45"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O1" activeCellId="0" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.8125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6280,17 +6280,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AF46"/>
+  <dimension ref="A1:S46"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M41" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AB50" activeCellId="0" sqref="AB50"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.37109375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="31.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="26.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="1" width="38.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="38.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16372" style="0" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="120.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6351,45 +6352,6 @@
       <c r="S1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="T1" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="U1" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="V1" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="W1" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="X1" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="Y1" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="Z1" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="AA1" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB1" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="AC1" s="7" t="s">
-        <v>262</v>
-      </c>
-      <c r="AD1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="AE1" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="AF1" s="5" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="59" t="s">
@@ -6401,7 +6363,7 @@
       <c r="C2" s="60" t="s">
         <v>264</v>
       </c>
-      <c r="AB2" s="61" t="s">
+      <c r="O2" s="61" t="s">
         <v>265</v>
       </c>
     </row>
@@ -6415,7 +6377,7 @@
       <c r="C3" s="60" t="s">
         <v>267</v>
       </c>
-      <c r="AB3" s="62" t="s">
+      <c r="O3" s="62" t="s">
         <v>268</v>
       </c>
     </row>
@@ -6429,7 +6391,7 @@
       <c r="C4" s="60" t="s">
         <v>270</v>
       </c>
-      <c r="AB4" s="62" t="s">
+      <c r="O4" s="62" t="s">
         <v>268</v>
       </c>
     </row>
@@ -6443,7 +6405,7 @@
       <c r="C5" s="60" t="s">
         <v>272</v>
       </c>
-      <c r="AB5" s="59" t="s">
+      <c r="O5" s="59" t="s">
         <v>273</v>
       </c>
     </row>
@@ -6457,7 +6419,7 @@
       <c r="C6" s="60" t="s">
         <v>275</v>
       </c>
-      <c r="AB6" s="59" t="s">
+      <c r="O6" s="59" t="s">
         <v>276</v>
       </c>
     </row>
@@ -6471,7 +6433,7 @@
       <c r="C7" s="60" t="s">
         <v>278</v>
       </c>
-      <c r="AB7" s="59" t="s">
+      <c r="O7" s="59" t="s">
         <v>279</v>
       </c>
     </row>
@@ -6485,7 +6447,7 @@
       <c r="C8" s="60" t="s">
         <v>281</v>
       </c>
-      <c r="AB8" s="59" t="s">
+      <c r="O8" s="59" t="s">
         <v>273</v>
       </c>
     </row>
@@ -6499,7 +6461,7 @@
       <c r="C9" s="60" t="s">
         <v>283</v>
       </c>
-      <c r="AB9" s="59" t="s">
+      <c r="O9" s="59" t="s">
         <v>284</v>
       </c>
     </row>
@@ -6513,7 +6475,7 @@
       <c r="C10" s="60" t="s">
         <v>286</v>
       </c>
-      <c r="AB10" s="61" t="s">
+      <c r="O10" s="61" t="s">
         <v>287</v>
       </c>
     </row>
@@ -6527,7 +6489,7 @@
       <c r="C11" s="60" t="s">
         <v>290</v>
       </c>
-      <c r="AB11" s="59" t="s">
+      <c r="O11" s="59" t="s">
         <v>291</v>
       </c>
     </row>
@@ -6541,7 +6503,7 @@
       <c r="C12" s="60" t="s">
         <v>293</v>
       </c>
-      <c r="AB12" s="59" t="s">
+      <c r="O12" s="59" t="s">
         <v>294</v>
       </c>
     </row>
@@ -6555,7 +6517,7 @@
       <c r="C13" s="60" t="s">
         <v>296</v>
       </c>
-      <c r="AB13" s="59" t="s">
+      <c r="O13" s="59" t="s">
         <v>294</v>
       </c>
     </row>
@@ -6569,7 +6531,7 @@
       <c r="C14" s="60" t="s">
         <v>298</v>
       </c>
-      <c r="AB14" s="59" t="s">
+      <c r="O14" s="59" t="s">
         <v>299</v>
       </c>
     </row>
@@ -6583,7 +6545,7 @@
       <c r="C15" s="60" t="s">
         <v>301</v>
       </c>
-      <c r="AB15" s="59" t="s">
+      <c r="O15" s="59" t="s">
         <v>302</v>
       </c>
     </row>
@@ -6597,7 +6559,7 @@
       <c r="C16" s="60" t="s">
         <v>304</v>
       </c>
-      <c r="AB16" s="59" t="s">
+      <c r="O16" s="59" t="s">
         <v>305</v>
       </c>
     </row>
@@ -6611,7 +6573,7 @@
       <c r="C17" s="60" t="s">
         <v>307</v>
       </c>
-      <c r="AB17" s="59" t="s">
+      <c r="O17" s="59" t="s">
         <v>308</v>
       </c>
     </row>
@@ -6625,7 +6587,7 @@
       <c r="C18" s="60" t="s">
         <v>310</v>
       </c>
-      <c r="AB18" s="61" t="s">
+      <c r="O18" s="61" t="s">
         <v>311</v>
       </c>
     </row>
@@ -6639,7 +6601,7 @@
       <c r="C19" s="60" t="s">
         <v>313</v>
       </c>
-      <c r="AB19" s="59" t="s">
+      <c r="O19" s="59" t="s">
         <v>314</v>
       </c>
     </row>
@@ -6653,7 +6615,7 @@
       <c r="C20" s="60" t="s">
         <v>316</v>
       </c>
-      <c r="AB20" s="59" t="s">
+      <c r="O20" s="59" t="s">
         <v>317</v>
       </c>
     </row>
@@ -6667,7 +6629,7 @@
       <c r="C21" s="60" t="s">
         <v>320</v>
       </c>
-      <c r="AB21" s="62" t="s">
+      <c r="O21" s="62" t="s">
         <v>321</v>
       </c>
     </row>
@@ -6681,7 +6643,7 @@
       <c r="C22" s="60" t="s">
         <v>323</v>
       </c>
-      <c r="AB22" s="59" t="s">
+      <c r="O22" s="59" t="s">
         <v>324</v>
       </c>
     </row>
@@ -6695,7 +6657,7 @@
       <c r="C23" s="60" t="s">
         <v>326</v>
       </c>
-      <c r="AB23" s="63" t="s">
+      <c r="O23" s="63" t="s">
         <v>327</v>
       </c>
     </row>
@@ -6709,7 +6671,7 @@
       <c r="C24" s="60" t="s">
         <v>329</v>
       </c>
-      <c r="AB24" s="59" t="s">
+      <c r="O24" s="59" t="s">
         <v>330</v>
       </c>
     </row>
@@ -6723,7 +6685,7 @@
       <c r="C25" s="60" t="s">
         <v>332</v>
       </c>
-      <c r="AB25" s="63" t="s">
+      <c r="O25" s="63" t="s">
         <v>321</v>
       </c>
     </row>
@@ -6737,7 +6699,7 @@
       <c r="C26" s="60" t="s">
         <v>334</v>
       </c>
-      <c r="AB26" s="59" t="s">
+      <c r="O26" s="59" t="s">
         <v>308</v>
       </c>
     </row>
@@ -6751,7 +6713,7 @@
       <c r="C27" s="60" t="s">
         <v>336</v>
       </c>
-      <c r="AB27" s="59" t="s">
+      <c r="O27" s="59" t="s">
         <v>337</v>
       </c>
     </row>
@@ -6765,7 +6727,7 @@
       <c r="C28" s="60" t="s">
         <v>339</v>
       </c>
-      <c r="AB28" s="61" t="s">
+      <c r="O28" s="61" t="s">
         <v>340</v>
       </c>
     </row>
@@ -6779,7 +6741,7 @@
       <c r="C29" s="60" t="s">
         <v>342</v>
       </c>
-      <c r="AB29" s="59" t="s">
+      <c r="O29" s="59" t="s">
         <v>308</v>
       </c>
     </row>
@@ -6793,7 +6755,7 @@
       <c r="C30" s="60" t="s">
         <v>344</v>
       </c>
-      <c r="AB30" s="59" t="s">
+      <c r="O30" s="59" t="s">
         <v>345</v>
       </c>
     </row>
@@ -6807,7 +6769,7 @@
       <c r="C31" s="60" t="s">
         <v>347</v>
       </c>
-      <c r="AB31" s="59" t="s">
+      <c r="O31" s="59" t="s">
         <v>345</v>
       </c>
     </row>
@@ -6821,7 +6783,7 @@
       <c r="C32" s="60" t="s">
         <v>349</v>
       </c>
-      <c r="AB32" s="59" t="s">
+      <c r="O32" s="59" t="s">
         <v>345</v>
       </c>
     </row>
@@ -6835,7 +6797,7 @@
       <c r="C33" s="60" t="s">
         <v>351</v>
       </c>
-      <c r="AB33" s="59" t="s">
+      <c r="O33" s="59" t="s">
         <v>345</v>
       </c>
     </row>
@@ -6849,7 +6811,7 @@
       <c r="C34" s="60" t="s">
         <v>354</v>
       </c>
-      <c r="AB34" s="59"/>
+      <c r="O34" s="59"/>
     </row>
     <row r="35" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="59" t="s">
@@ -6883,7 +6845,7 @@
       <c r="C37" s="60" t="s">
         <v>360</v>
       </c>
-      <c r="AB37" s="59" t="s">
+      <c r="O37" s="59" t="s">
         <v>361</v>
       </c>
     </row>
@@ -6897,7 +6859,7 @@
       <c r="C38" s="60" t="s">
         <v>362</v>
       </c>
-      <c r="AB38" s="61" t="s">
+      <c r="O38" s="61" t="s">
         <v>363</v>
       </c>
     </row>
@@ -6911,7 +6873,7 @@
       <c r="C39" s="60" t="s">
         <v>365</v>
       </c>
-      <c r="AB39" s="59" t="s">
+      <c r="O39" s="59" t="s">
         <v>345</v>
       </c>
     </row>
@@ -6925,7 +6887,7 @@
       <c r="C40" s="60" t="s">
         <v>367</v>
       </c>
-      <c r="AB40" s="59" t="s">
+      <c r="O40" s="59" t="s">
         <v>345</v>
       </c>
     </row>
@@ -6939,7 +6901,7 @@
       <c r="C41" s="60" t="s">
         <v>369</v>
       </c>
-      <c r="AB41" s="61" t="s">
+      <c r="O41" s="61" t="s">
         <v>370</v>
       </c>
     </row>
@@ -6953,7 +6915,7 @@
       <c r="C42" s="60" t="s">
         <v>371</v>
       </c>
-      <c r="AB42" s="59" t="s">
+      <c r="O42" s="59" t="s">
         <v>372</v>
       </c>
     </row>
@@ -6967,7 +6929,7 @@
       <c r="C43" s="60" t="s">
         <v>373</v>
       </c>
-      <c r="AB43" s="59" t="s">
+      <c r="O43" s="59" t="s">
         <v>374</v>
       </c>
     </row>
@@ -6981,7 +6943,7 @@
       <c r="C44" s="60" t="s">
         <v>375</v>
       </c>
-      <c r="AB44" s="59" t="s">
+      <c r="O44" s="59" t="s">
         <v>374</v>
       </c>
     </row>
@@ -6995,42 +6957,42 @@
       <c r="C45" s="60" t="s">
         <v>376</v>
       </c>
-      <c r="AB45" s="59" t="s">
+      <c r="O45" s="59" t="s">
         <v>377</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AB46" s="61"/>
+      <c r="O46" s="61"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="AB2" r:id="rId1" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
-    <hyperlink ref="AB5" r:id="rId2" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
-    <hyperlink ref="AB8" r:id="rId3" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
-    <hyperlink ref="AB9" r:id="rId4" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
-    <hyperlink ref="AB15" r:id="rId5" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
-    <hyperlink ref="AB16" r:id="rId6" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
-    <hyperlink ref="AB17" r:id="rId7" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
-    <hyperlink ref="AB18" r:id="rId8" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
-    <hyperlink ref="AB19" r:id="rId9" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
-    <hyperlink ref="AB20" r:id="rId10" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
-    <hyperlink ref="AB26" r:id="rId11" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
-    <hyperlink ref="AB27" r:id="rId12" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
-    <hyperlink ref="AB28" r:id="rId13" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
-    <hyperlink ref="AB29" r:id="rId14" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
-    <hyperlink ref="AB30" r:id="rId15" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
-    <hyperlink ref="AB31" r:id="rId16" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
-    <hyperlink ref="AB32" r:id="rId17" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
-    <hyperlink ref="AB33" r:id="rId18" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
-    <hyperlink ref="AB37" r:id="rId19" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
-    <hyperlink ref="AB38" r:id="rId20" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
-    <hyperlink ref="AB39" r:id="rId21" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
-    <hyperlink ref="AB40" r:id="rId22" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
-    <hyperlink ref="AB41" r:id="rId23" location="Kraftwerke" display="&lt;sup&gt;b&lt;/sup&gt; Greenhouse gas potential during the usage phase was calculated based on emission factors for the German electricity mix provided by the Federal Environment Agency for the year 2022 (https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke);"/>
-    <hyperlink ref="AB42" r:id="rId24" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
-    <hyperlink ref="AB43" r:id="rId25" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
-    <hyperlink ref="AB44" r:id="rId26" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
-    <hyperlink ref="AB45" r:id="rId27" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
+    <hyperlink ref="O2" r:id="rId1" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
+    <hyperlink ref="O5" r:id="rId2" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
+    <hyperlink ref="O8" r:id="rId3" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
+    <hyperlink ref="O9" r:id="rId4" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
+    <hyperlink ref="O15" r:id="rId5" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
+    <hyperlink ref="O16" r:id="rId6" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
+    <hyperlink ref="O17" r:id="rId7" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
+    <hyperlink ref="O18" r:id="rId8" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
+    <hyperlink ref="O19" r:id="rId9" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
+    <hyperlink ref="O20" r:id="rId10" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
+    <hyperlink ref="O26" r:id="rId11" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
+    <hyperlink ref="O27" r:id="rId12" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
+    <hyperlink ref="O28" r:id="rId13" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
+    <hyperlink ref="O29" r:id="rId14" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
+    <hyperlink ref="O30" r:id="rId15" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
+    <hyperlink ref="O31" r:id="rId16" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
+    <hyperlink ref="O32" r:id="rId17" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
+    <hyperlink ref="O33" r:id="rId18" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
+    <hyperlink ref="O37" r:id="rId19" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
+    <hyperlink ref="O38" r:id="rId20" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
+    <hyperlink ref="O39" r:id="rId21" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
+    <hyperlink ref="O40" r:id="rId22" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
+    <hyperlink ref="O41" r:id="rId23" location="Kraftwerke" display="&lt;sup&gt;b&lt;/sup&gt; Greenhouse gas potential during the usage phase was calculated based on emission factors for the German electricity mix provided by the Federal Environment Agency for the year 2022 (https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke);"/>
+    <hyperlink ref="O42" r:id="rId24" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
+    <hyperlink ref="O43" r:id="rId25" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
+    <hyperlink ref="O44" r:id="rId26" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
+    <hyperlink ref="O45" r:id="rId27" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
implemented appearance of superscripts
</commit_message>
<xml_diff>
--- a/02_work_doc/01_daten/12_component_list/componentList_oneSheet.xlsx
+++ b/02_work_doc/01_daten/12_component_list/componentList_oneSheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="German" sheetId="1" state="visible" r:id="rId3"/>
@@ -3891,7 +3891,7 @@
   </sheetPr>
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="O1" activeCellId="0" sqref="O1"/>
     </sheetView>
   </sheetViews>
@@ -6282,7 +6282,7 @@
   </sheetPr>
   <dimension ref="A1:S46"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
translated the explanation text in component list
</commit_message>
<xml_diff>
--- a/02_work_doc/01_daten/12_component_list/componentList_oneSheet.xlsx
+++ b/02_work_doc/01_daten/12_component_list/componentList_oneSheet.xlsx
@@ -2412,6 +2412,69 @@
     <t xml:space="preserve">Humidity sensor module for use in HVAC systems to measure relative humidity and temperature with high accuracy and short response time. Measures humidity from 0-100%. Includes connections for power supply and BUS system via cable.</t>
   </si>
   <si>
+    <t xml:space="preserve">&lt;sup&gt;a&lt;/sup&gt;Product packaging is included; for the THP, only the mass balance was used, production processes and their energy consumption were not considered due to a lack of data; the calculation was performed using the CML-IA Baseline 3.08 method.
+&lt;sup&gt;b&lt;/sup&gt;Greenhouse gas potential during the usage phase was calculated based on the emission factors for the German electricity mix from the Federal Environment Agency for the year 2022 (https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke);
+&lt;sup&gt;c&lt;/sup&gt;Assumption of operating time: 24h/day.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Presence Detector</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Presence detector that detects the movement of people in a room to control indoor lighting.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;sup&gt;a&lt;/sup&gt;Packaging is included, European electricity mix;
+&lt;sup&gt;b&lt;/sup&gt;Operating time: Assumption = 30% active; 70% passive.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Light Sensor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sunlight sensor used as a probe in HVAC systems where solar radiation compensation is planned. The probe uses a solar cell to detect sunlight and generates a radiation-dependent current that is evaluated by the sensor.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;sup&gt;a&lt;/sup&gt;Product packaging is included; for the THP, only the mass balance was used, production processes and their energy consumption were not considered due to a lack of data; the calculation was performed using the CML-IA Baseline 3.08 method.
+&lt;sup&gt;b&lt;/sup&gt;The light sensor is equipped with a solar module and requires no external energy during the usage phase;
+&lt;sup&gt;c&lt;/sup&gt;An operating time of 12 hours per day is assumed (average daylight time per year).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Water Meter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Conventional water meter for physical measurement of cold/hot water consumption. The meter consists of a flow element, a counter, and a display. Flow rate: 4 m³/h.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Heat Meter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ultrasonic heat and cooling energy meter for measuring flow and energy in heating or cooling circuits. Flow rate: 25 m³/h.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;sup&gt;a&lt;/sup&gt;Product packaging is included; for the THP, only the mass balance was used, production processes and their energy consumption were not considered due to a lack of data; the calculation was performed using the CML-IA Baseline 3.08 method.
+&lt;sup&gt;b&lt;/sup&gt;Greenhouse gas potential during the usage phase was calculated based on the emission factors for the German electricity mix from the Federal Environment Agency for the year 2022 (https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke);
+&lt;sup&gt;c&lt;/sup&gt;Assumed operating time: 24h/day.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flow Meter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ultrasonic flow sensor with a maximum flow rate of 12 m³/h (volume flow meter).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;sup&gt;a&lt;/sup&gt;Product packaging is included; for the THP, only the mass balance was used, production processes and their energy consumption were not considered due to a lack of data; the calculation was performed using the CML-IA Baseline 3.08 method.
+&lt;sup&gt;b&lt;/sup&gt;No data is available for the electrical power, so no greenhouse gas potential could be calculated for the usage phase;
+&lt;sup&gt;c&lt;/sup&gt;Assumed operating time: 24h/day.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actuator Technology</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Small Fan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Central ventilation system for supply or exhaust air with a capacity of 5000 m³/h. It is a fan installed on the roof or beside the building, housed in a galvanized steel casing.</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="10"/>
@@ -2419,8 +2482,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">&lt;sup&gt;a&lt;/sup&gt;Product packaging is included; for the THP, only the mass balance was used, production processes and their energy consumption were not considered due to a lack of data; the calculation was performed using the CML-IA Baseline 3.08 method.
-&lt;sup&gt;b&lt;/sup&gt;Greenhouse gas potential during the usage phase was calculated based on the emission factors for the German electricity mix from the Federal Environment Agency for the year 2022 (</t>
+      <t xml:space="preserve">&lt;sup&gt;a&lt;/sup&gt;Fan for commercial and light industrial applications, performance calculation by interpolating the values from: </t>
     </r>
     <r>
       <rPr>
@@ -2430,7 +2492,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke</t>
+      <t xml:space="preserve">https://www.dasslerventilatoren.info/contents/de/d135_WandventilatorECMotor.html</t>
     </r>
     <r>
       <rPr>
@@ -2439,53 +2501,9 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">);
-&lt;sup&gt;c&lt;/sup&gt;Assumption of operating time: 24h/day.</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Presence Detector</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Presence detector that detects the movement of people in a room to control indoor lighting.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;sup&gt;a&lt;/sup&gt;Packaging is included, European electricity mix;
-&lt;sup&gt;b&lt;/sup&gt;Operating time: Assumption = 30% active; 70% passive.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Light Sensor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sunlight sensor used as a probe in HVAC systems where solar radiation compensation is planned. The probe uses a solar cell to detect sunlight and generates a radiation-dependent current that is evaluated by the sensor.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;sup&gt;a&lt;/sup&gt;Product packaging is included; for the THP, only the mass balance was used, production processes and their energy consumption were not considered due to a lack of data; the calculation was performed using the CML-IA Baseline 3.08 method.
-&lt;sup&gt;b&lt;/sup&gt;The light sensor is equipped with a solar module and requires no external energy during the usage phase;
-&lt;sup&gt;c&lt;/sup&gt;An operating time of 12 hours per day is assumed (average daylight time per year).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Water Meter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Conventional water meter for physical measurement of cold/hot water consumption. The meter consists of a flow element, a counter, and a display. Flow rate: 4 m³/h.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Heat Meter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ultrasonic heat and cooling energy meter for measuring flow and energy in heating or cooling circuits. Flow rate: 25 m³/h.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">&lt;sup&gt;a&lt;/sup&gt;Product packaging is included; for the THP, only the mass balance was used, production processes and their energy consumption were not considered due to a lack of data; the calculation was performed using the CML-IA Baseline 3.08 method.
-&lt;sup&gt;b&lt;/sup&gt;Greenhouse gas potential during the usage phase was calculated based on the emission factors for the German electricity mix from the Federal Environment Agency for the year 2022 (</t>
+      <t xml:space="preserve">; higher power outputs are possible depending on the application.
+&lt;sup&gt;b&lt;/sup&gt;A daily usage time from 8 AM to 6 PM is assumed.
+&lt;sup&gt;c&lt;/sup&gt;Greenhouse gas potential during the usage phase was calculated based on the emission factors for the German electricity mix from the Federal Environment Agency for the year 2022 (</t>
     </r>
     <r>
       <rPr>
@@ -2505,28 +2523,14 @@
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">);
-&lt;sup&gt;c&lt;/sup&gt;Assumed operating time: 24h/day.</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Flow Meter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ultrasonic flow sensor with a maximum flow rate of 12 m³/h (volume flow meter).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;sup&gt;a&lt;/sup&gt;Product packaging is included; for the THP, only the mass balance was used, production processes and their energy consumption were not considered due to a lack of data; the calculation was performed using the CML-IA Baseline 3.08 method.
-&lt;sup&gt;b&lt;/sup&gt;No data is available for the electrical power, so no greenhouse gas potential could be calculated for the usage phase;
-&lt;sup&gt;c&lt;/sup&gt;Assumed operating time: 24h/day.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Actuator Technology</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Small Fan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Central ventilation system for supply or exhaust air with a capacity of 5000 m³/h. It is a fan installed on the roof or beside the building, housed in a galvanized steel casing.</t>
+Assumed operating time: 10 hours per day.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Medium Fan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Central ventilation system for supply or exhaust air with a capacity of 10,000 m³/h. It is a fan installed on the roof or beside the building, housed in a galvanized steel casing.</t>
   </si>
   <si>
     <r>
@@ -2536,7 +2540,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">&lt;sup&gt;a&lt;/sup&gt;Fan for commercial and light industrial applications, performance calculation by interpolating the values from: </t>
+      <t xml:space="preserve">&lt;sup&gt;a&lt;/sup&gt;Fan for commercial and light industrial applications, performance calculated by interpolating the values from: </t>
     </r>
     <r>
       <rPr>
@@ -2557,7 +2561,25 @@
       </rPr>
       <t xml:space="preserve">; higher power outputs are possible depending on the application.
 &lt;sup&gt;b&lt;/sup&gt;A daily usage time from 8 AM to 6 PM is assumed.
-&lt;sup&gt;c&lt;/sup&gt;Greenhouse gas potential during the usage phase was calculated based on the emission factors for the German electricity mix from the Federal Environment Agency for the year 2022 (</t>
+&lt;sup&gt;c&lt;/sup&gt;Greenhouse gas potential during the usage phase was calculated based on the emission factors for the German electricity mix from the Federal Environment Agency for the year 2022 (https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke);
+Assumed operating time: 10 hours per day.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Large Fan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Central ventilation system for supply or exhaust air with a capacity of 30,000 m³/h. It is a fan installed on the roof or beside the building, housed in a galvanized steel casing.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">&lt;sup&gt;a&lt;/sup&gt;Fan for commercial and light industrial applications, performance calculated by interpolating the values from: </t>
     </r>
     <r>
       <rPr>
@@ -2567,7 +2589,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke</t>
+      <t xml:space="preserve">https://www.dasslerventilatoren.info/contents/de/d135_WandventilatorECMotor.html</t>
     </r>
     <r>
       <rPr>
@@ -2576,25 +2598,9 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">);
-Assumed operating time: 10 hours per day.</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Medium Fan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Central ventilation system for supply or exhaust air with a capacity of 10,000 m³/h. It is a fan installed on the roof or beside the building, housed in a galvanized steel casing.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">&lt;sup&gt;a&lt;/sup&gt;Fan for commercial and light industrial applications, performance calculated by interpolating the values from: </t>
+      <t xml:space="preserve">; higher power outputs are possible depending on the application.
+&lt;sup&gt;b&lt;/sup&gt;A daily usage time from 8 AM to 6 PM is assumed.
+&lt;sup&gt;c&lt;/sup&gt;Greenhouse gas potential during the usage phase was calculated based on the emission factors for the German electricity mix from the Federal Environment Agency for the year 2022 (</t>
     </r>
     <r>
       <rPr>
@@ -2604,7 +2610,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">https://www.dasslerventilatoren.info/contents/de/d135_WandventilatorECMotor.html</t>
+      <t xml:space="preserve">https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke</t>
     </r>
     <r>
       <rPr>
@@ -2613,38 +2619,11 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">; higher power outputs are possible depending on the application.
-&lt;sup&gt;b&lt;/sup&gt;A daily usage time from 8 AM to 6 PM is assumed.
-&lt;sup&gt;c&lt;/sup&gt;Greenhouse gas potential during the usage phase was calculated based on the emission factors for the German electricity mix from the Federal Environment Agency for the year 2022 (</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
       <t xml:space="preserve">);
 Assumed operating time: 10 hours per day.</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Large Fan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Central ventilation system for supply or exhaust air with a capacity of 30,000 m³/h. It is a fan installed on the roof or beside the building, housed in a galvanized steel casing.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Volume Flow Controller</t>
   </si>
   <si>
@@ -2661,36 +2640,9 @@
     <t xml:space="preserve">Circulation pump with a power rating of 50-250 W for heating systems.</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">&lt;sup&gt;b&lt;/sup&gt;Greenhouse gas potential during the usage phase was calculated based on the emission factors for the German electricity mix from the Federal Environment Agency for the year 2022 (</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">);
+    <t xml:space="preserve">&lt;sup&gt;b&lt;/sup&gt;Greenhouse gas potential during the usage phase was calculated based on the emission factors for the German electricity mix from the Federal Environment Agency for the year 2022 (https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke);
 &lt;sup&gt;a&lt;/sup&gt;Assumed operating time: 3,000 hours per year (range: 2,000 to 4,000 hours);
 &lt;sup&gt;c&lt;/sup&gt;The circulation pump has a power rating of 50-250W; for the calculation, an effective power of 150W is assumed.</t>
-    </r>
   </si>
   <si>
     <t xml:space="preserve">Small Electric Valve Actuator</t>
@@ -2699,37 +2651,10 @@
     <t xml:space="preserve">Small electric valve actuator for controlling water-side regulation of hot and cooling water in HVAC systems. Automatic detection of valve stroke. Includes manual adjuster and position indicator.</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">&lt;sup&gt;a&lt;/sup&gt;Product packaging is included; for the THP, only the mass balance was used, production processes and their energy consumption were not considered due to a lack of data; the calculation was performed using the CML-IA Baseline 3.08 method.
-&lt;sup&gt;b&lt;/sup&gt;Greenhouse gas potential during the usage phase was calculated based on the emission factors for the German electricity mix from the Federal Environment Agency for the year 2022 (</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">);
+    <t xml:space="preserve">&lt;sup&gt;a&lt;/sup&gt;Product packaging is included; for the THP, only the mass balance was used, production processes and their energy consumption were not considered due to a lack of data; the calculation was performed using the CML-IA Baseline 3.08 method.
+&lt;sup&gt;b&lt;/sup&gt;Greenhouse gas potential during the usage phase was calculated based on the emission factors for the German electricity mix from the Federal Environment Agency for the year 2022 (https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke);
 The lifespan of the actuator is assumed to be 15 years (typical lifespan of a seal);
 &lt;sup&gt;c&lt;/sup&gt;The operating time of the actuator is 876 hours.</t>
-    </r>
   </si>
   <si>
     <t xml:space="preserve">Large Electric Valve Actuator</t>
@@ -2738,35 +2663,8 @@
     <t xml:space="preserve">Electric actuator for operating two-way and three-way valves with a 20mm stroke as control and shut-off devices in HVAC systems. Includes manual adjuster, position, and status indicator.</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">&lt;sup&gt;a&lt;/sup&gt;Product packaging is included; for the THP, only the mass balance was used, production processes and their energy consumption were not considered due to a lack of data; the calculation was performed using the CML-IA Baseline 3.08 method.
-&lt;sup&gt;b&lt;/sup&gt;Greenhouse gas potential during the usage phase was calculated based on the emission factors for the German electricity mix from the Federal Environment Agency for the year 2022 (</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">).</t>
-    </r>
+    <t xml:space="preserve">&lt;sup&gt;a&lt;/sup&gt;Product packaging is included; for the THP, only the mass balance was used, production processes and their energy consumption were not considered due to a lack of data; the calculation was performed using the CML-IA Baseline 3.08 method.
+&lt;sup&gt;b&lt;/sup&gt;Greenhouse gas potential during the usage phase was calculated based on the emission factors for the German electricity mix from the Federal Environment Agency for the year 2022 (https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke).</t>
   </si>
   <si>
     <t xml:space="preserve">BUS System: KNX Sunshade Actuator</t>
@@ -2786,36 +2684,9 @@
     <t xml:space="preserve">Switch/dimmer actuator used for switching, dimming, and scene control (e.g., LED) in building automation. Device control is via KNX.</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">&lt;sup&gt;a&lt;/sup&gt;Product packaging is included; for the THP, only the mass balance was used, production processes and their energy consumption were not considered due to a lack of data; the calculation was performed using the CML-IA Baseline 3.08 method.
-&lt;sup&gt;b&lt;/sup&gt;Greenhouse gas potential during the usage phase was calculated based on the emission factors for the German electricity mix from the Federal Environment Agency for the year 2022 (</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">).
+    <t xml:space="preserve">&lt;sup&gt;a&lt;/sup&gt;Product packaging is included; for the THP, only the mass balance was used, production processes and their energy consumption were not considered due to a lack of data; the calculation was performed using the CML-IA Baseline 3.08 method.
+&lt;sup&gt;b&lt;/sup&gt;Greenhouse gas potential during the usage phase was calculated based on the emission factors for the German electricity mix from the Federal Environment Agency for the year 2022 (https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke).
 &lt;sup&gt;c&lt;/sup&gt;An operating time of 16 hours per day is assumed (average wake time).</t>
-    </r>
   </si>
   <si>
     <t xml:space="preserve">BUS System: KNX Thermo Actuator</t>
@@ -2824,36 +2695,9 @@
     <t xml:space="preserve">Thermo actuator with 2 outputs for controlling electrothermal actuators in heating or cooling systems.</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">&lt;sup&gt;a&lt;/sup&gt;Product packaging is included; for the THP, only the mass balance was used, production processes and their energy consumption were not considered due to a lack of data; the calculation was performed using the CML-IA Baseline 3.08 method.
-&lt;sup&gt;b&lt;/sup&gt;Greenhouse gas potential during the usage phase was calculated based on the emission factors for the German electricity mix from the Federal Environment Agency for the year 2022 (</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">).
+    <t xml:space="preserve">&lt;sup&gt;a&lt;/sup&gt;Product packaging is included; for the THP, only the mass balance was used, production processes and their energy consumption were not considered due to a lack of data; the calculation was performed using the CML-IA Baseline 3.08 method.
+&lt;sup&gt;b&lt;/sup&gt;Greenhouse gas potential during the usage phase was calculated based on the emission factors for the German electricity mix from the Federal Environment Agency for the year 2022 (https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke).
 &lt;sup&gt;c&lt;/sup&gt;An operating time of 24 hours per day is assumed.</t>
-    </r>
   </si>
   <si>
     <t xml:space="preserve">Signal Processing</t>
@@ -2914,36 +2758,9 @@
     <t xml:space="preserve">Interface between KNX and DALI. Up to 64 DALI actuators and additional sensors can be connected per channel.</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">&lt;sup&gt;a&lt;/sup&gt;Product packaging is included; for the THP, only the mass balance was used, production processes and their energy consumption were not considered due to a lack of data; the calculation was performed using the CML-IA Baseline 3.08 method.
-&lt;sup&gt;b&lt;/sup&gt;Greenhouse gas potential during the usage phase was calculated based on the emission factors for the German electricity mix from the Federal Environment Agency for the year 2022 (</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">).
+    <t xml:space="preserve">&lt;sup&gt;a&lt;/sup&gt;Product packaging is included; for the THP, only the mass balance was used, production processes and their energy consumption were not considered due to a lack of data; the calculation was performed using the CML-IA Baseline 3.08 method.
+&lt;sup&gt;b&lt;/sup&gt;Greenhouse gas potential during the usage phase was calculated based on the emission factors for the German electricity mix from the Federal Environment Agency for the year 2022 (https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke).
 &lt;sup&gt;c&lt;/sup&gt;It is assumed that the BACnet and DALI interfaces have similar energy consumption values.</t>
-    </r>
   </si>
   <si>
     <t xml:space="preserve">BUS System: KNX IP Router Interface</t>
@@ -2952,53 +2769,22 @@
     <t xml:space="preserve">IP router that connects KNX lines via data networks using the Internet Protocol and the KNXnet/IP standard. This device also allows bus access from a PC or other data processing devices.</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;sup&gt;a&lt;/sup&gt;Product packaging is included; for the THP, only the mass balance was used, production processes and their energy consumption were not considered due to a lack of data; the calculation was performed using the CML-IA Baseline 3.08 method.
+    <t xml:space="preserve">BUS System: KNX IP Control Center</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Web server component integrated for operation, monitoring, and programming of KNX systems. Standard web browsers can display and visually represent control pages. The component provides an interface to KNX installations via IP data networks.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BUS System: KNX Web Server</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Web server enabling remote control and monitoring of systems via web and smartphone app.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;sup&gt;a&lt;/sup&gt;Product packaging is included; for the THP, only the mass balance was used. Production processes and their energy consumption were not considered due to a lack of data; the calculation was performed using the CML-IA Baseline 3.08 method.
 &lt;sup&gt;b&lt;/sup&gt;Greenhouse gas potential during the usage phase was calculated based on the emission factors for the German electricity mix from the Federal Environment Agency for the year 2022 (https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke).</t>
   </si>
   <si>
-    <t xml:space="preserve">BUS System: KNX IP Control Center</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Web server component integrated for operation, monitoring, and programming of KNX systems. Standard web browsers can display and visually represent control pages. The component provides an interface to KNX installations via IP data networks.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BUS System: KNX Web Server</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Web server enabling remote control and monitoring of systems via web and smartphone app.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">&lt;sup&gt;a&lt;/sup&gt;Product packaging is included; for the THP, only the mass balance was used. Production processes and their energy consumption were not considered due to a lack of data; the calculation was performed using the CML-IA Baseline 3.08 method.
-&lt;sup&gt;b&lt;/sup&gt;Greenhouse gas potential during the usage phase was calculated based on the emission factors for the German electricity mix from the Federal Environment Agency for the year 2022 (</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">).</t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve">BUS System: KNX Repeater</t>
   </si>
   <si>
@@ -3044,36 +2830,9 @@
     <t xml:space="preserve">Household Ferraris-type electricity meter.</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">&lt;sup&gt;a&lt;/sup&gt;An operating time of 24 hours per day was assumed.
-&lt;sup&gt;b&lt;/sup&gt;Greenhouse gas potential during the usage phase was calculated based on the emission factors for the German electricity mix from the Federal Environment Agency for the year 2022 (</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">).
+    <t xml:space="preserve">&lt;sup&gt;a&lt;/sup&gt;An operating time of 24 hours per day was assumed.
+&lt;sup&gt;b&lt;/sup&gt;Greenhouse gas potential during the usage phase was calculated based on the emission factors for the German electricity mix from the Federal Environment Agency for the year 2022 (https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke).
 &lt;sup&gt;c&lt;/sup&gt;For the THP, only the mass balance was used. Production processes and their energy consumption were not considered due to a lack of data; the calculation was performed using the CML-IA Baseline 3.08 method.</t>
-    </r>
   </si>
   <si>
     <t xml:space="preserve">Smart meter electricity meter.</t>
@@ -3109,70 +2868,16 @@
     <t xml:space="preserve">Router for connecting to the internet from the Ecoinvent database. The product represents a Cisco Service Router 1800 Series with a maximum data rate of 100 Mbit/s and a realistic data rate of 25 Mbit/s.</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">&lt;sup&gt;b&lt;/sup&gt;Greenhouse gas potential during the usage phase was calculated based on the emission factors for the German electricity mix from the Federal Environment Agency for the year 2022 (</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">).
+    <t xml:space="preserve">&lt;sup&gt;b&lt;/sup&gt;Greenhouse gas potential during the usage phase was calculated based on the emission factors for the German electricity mix from the Federal Environment Agency for the year 2022 (https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke).
 &lt;sup&gt;a&lt;/sup&gt;An operating time of 24 hours per day was assumed.
 &lt;sup&gt;c&lt;/sup&gt;The router's power consumption is 105W with an effective data transfer rate of 25 Mbit/s.</t>
-    </r>
   </si>
   <si>
     <t xml:space="preserve">Desktop computer without monitor from the Ecoinvent database. The product represents a typical desktop computer with a Pentium 4, 2000 MHz processor speed, 40 GB RAM HDD, and 512 GB storage capacity.</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">&lt;sup&gt;a&lt;/sup&gt;An operating time of 24 hours per day is assumed for the measurement computer in its function.
-&lt;sup&gt;b&lt;/sup&gt;Greenhouse gas potential during the usage phase was calculated based on the emission factors for the German electricity mix from the Federal Environment Agency for the year 2022 (</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">).</t>
-    </r>
+    <t xml:space="preserve">&lt;sup&gt;a&lt;/sup&gt;An operating time of 24 hours per day is assumed for the measurement computer in its function.
+&lt;sup&gt;b&lt;/sup&gt;Greenhouse gas potential during the usage phase was calculated based on the emission factors for the German electricity mix from the Federal Environment Agency for the year 2022 (https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke).</t>
   </si>
   <si>
     <t xml:space="preserve">Laptop computer from the Ecoinvent database. The product represents a typical laptop with a Pentium 3, 600 MHz processor speed, 10 GB RAM, 128 GB storage capacity, and a 12.1-inch screen.</t>
@@ -3181,35 +2886,8 @@
     <t xml:space="preserve">Thin-film transistor LCD display for a desktop computer. The product includes all display components, including electronics, frame, and energy consumption during manufacturing.</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">&lt;sup&gt;b&lt;/sup&gt;Greenhouse gas potential during the usage phase was calculated based on the emission factors for the German electricity mix from the Federal Environment Agency for the year 2022 (</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">).
+    <t xml:space="preserve">&lt;sup&gt;b&lt;/sup&gt;Greenhouse gas potential during the usage phase was calculated based on the emission factors for the German electricity mix from the Federal Environment Agency for the year 2022 (https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke).
 &lt;sup&gt;a&lt;/sup&gt;The monitor of the measurement computer is used only during working hours: 250 days/year * 8 hours = 2000 hours.</t>
-    </r>
   </si>
 </sst>
 </file>
@@ -3290,6 +2968,7 @@
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -3303,6 +2982,7 @@
       <color rgb="FF0000FF"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -3449,7 +3129,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="65">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3702,6 +3382,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3891,7 +3575,7 @@
   </sheetPr>
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="O1" activeCellId="0" sqref="O1"/>
     </sheetView>
   </sheetViews>
@@ -6291,7 +5975,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="31.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="26.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="38.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16372" style="0" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16372" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="120.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6353,7 +6037,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="59" t="s">
         <v>263</v>
       </c>
@@ -6395,7 +6079,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="59" t="s">
         <v>263</v>
       </c>
@@ -6405,7 +6089,7 @@
       <c r="C5" s="60" t="s">
         <v>272</v>
       </c>
-      <c r="O5" s="59" t="s">
+      <c r="O5" s="63" t="s">
         <v>273</v>
       </c>
     </row>
@@ -6437,7 +6121,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="59" t="s">
         <v>263</v>
       </c>
@@ -6447,11 +6131,11 @@
       <c r="C8" s="60" t="s">
         <v>281</v>
       </c>
-      <c r="O8" s="59" t="s">
+      <c r="O8" s="63" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="59" t="s">
         <v>263</v>
       </c>
@@ -6461,7 +6145,7 @@
       <c r="C9" s="60" t="s">
         <v>283</v>
       </c>
-      <c r="O9" s="59" t="s">
+      <c r="O9" s="63" t="s">
         <v>284</v>
       </c>
     </row>
@@ -6479,7 +6163,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="180.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="214.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="59" t="s">
         <v>288</v>
       </c>
@@ -6493,7 +6177,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="180.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="202.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="59" t="s">
         <v>288</v>
       </c>
@@ -6507,7 +6191,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="180.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="214.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="59" t="s">
         <v>288</v>
       </c>
@@ -6518,7 +6202,7 @@
         <v>296</v>
       </c>
       <c r="O13" s="59" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6526,214 +6210,214 @@
         <v>288</v>
       </c>
       <c r="B14" s="59" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="C14" s="60" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="O14" s="59" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="59" t="s">
         <v>288</v>
       </c>
       <c r="B15" s="59" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="C15" s="60" t="s">
-        <v>301</v>
-      </c>
-      <c r="O15" s="59" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="16" customFormat="false" ht="191.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O15" s="63" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="59" t="s">
         <v>288</v>
       </c>
       <c r="B16" s="59" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="C16" s="60" t="s">
-        <v>304</v>
-      </c>
-      <c r="O16" s="59" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="17" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O16" s="63" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="59" t="s">
         <v>288</v>
       </c>
       <c r="B17" s="59" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C17" s="60" t="s">
-        <v>307</v>
-      </c>
-      <c r="O17" s="59" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="18" customFormat="false" ht="180.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O17" s="63" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="59" t="s">
         <v>288</v>
       </c>
       <c r="B18" s="59" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="C18" s="60" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="O18" s="61" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="59" t="s">
         <v>288</v>
       </c>
       <c r="B19" s="59" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="C19" s="60" t="s">
-        <v>313</v>
-      </c>
-      <c r="O19" s="59" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="20" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O19" s="63" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="59" t="s">
         <v>288</v>
       </c>
       <c r="B20" s="59" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="C20" s="60" t="s">
-        <v>316</v>
-      </c>
-      <c r="O20" s="59" t="s">
         <v>317</v>
+      </c>
+      <c r="O20" s="63" t="s">
+        <v>318</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="59" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B21" s="59" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="C21" s="60" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="O21" s="62" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="59" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B22" s="59" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="C22" s="60" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="O22" s="59" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="59" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B23" s="59" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="C23" s="60" t="s">
-        <v>326</v>
-      </c>
-      <c r="O23" s="63" t="s">
         <v>327</v>
+      </c>
+      <c r="O23" s="64" t="s">
+        <v>328</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="59" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B24" s="59" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="C24" s="60" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="O24" s="59" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="59" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B25" s="59" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="C25" s="60" t="s">
-        <v>332</v>
-      </c>
-      <c r="O25" s="63" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>333</v>
+      </c>
+      <c r="O25" s="64" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="59" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B26" s="59" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="C26" s="60" t="s">
-        <v>334</v>
-      </c>
-      <c r="O26" s="59" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="180.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>335</v>
+      </c>
+      <c r="O26" s="63" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="59" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B27" s="59" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="C27" s="60" t="s">
-        <v>336</v>
-      </c>
-      <c r="O27" s="59" t="s">
         <v>337</v>
       </c>
-    </row>
-    <row r="28" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O27" s="63" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="59" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B28" s="59" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="C28" s="60" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="O28" s="61" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="59" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B29" s="59" t="s">
         <v>341</v>
@@ -6741,13 +6425,13 @@
       <c r="C29" s="60" t="s">
         <v>342</v>
       </c>
-      <c r="O29" s="59" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O29" s="63" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="59" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B30" s="59" t="s">
         <v>343</v>
@@ -6755,13 +6439,13 @@
       <c r="C30" s="60" t="s">
         <v>344</v>
       </c>
-      <c r="O30" s="59" t="s">
+      <c r="O30" s="63" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="59" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B31" s="59" t="s">
         <v>346</v>
@@ -6769,13 +6453,13 @@
       <c r="C31" s="60" t="s">
         <v>347</v>
       </c>
-      <c r="O31" s="59" t="s">
+      <c r="O31" s="63" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="59" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B32" s="59" t="s">
         <v>348</v>
@@ -6783,13 +6467,13 @@
       <c r="C32" s="60" t="s">
         <v>349</v>
       </c>
-      <c r="O32" s="59" t="s">
+      <c r="O32" s="63" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="59" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B33" s="59" t="s">
         <v>350</v>
@@ -6797,11 +6481,11 @@
       <c r="C33" s="60" t="s">
         <v>351</v>
       </c>
-      <c r="O33" s="59" t="s">
+      <c r="O33" s="63" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="59" t="s">
         <v>352</v>
       </c>
@@ -6835,7 +6519,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="59" t="s">
         <v>352</v>
       </c>
@@ -6845,11 +6529,11 @@
       <c r="C37" s="60" t="s">
         <v>360</v>
       </c>
-      <c r="O37" s="59" t="s">
+      <c r="O37" s="63" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="214.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="59" t="s">
         <v>352</v>
       </c>
@@ -6863,7 +6547,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="59" t="s">
         <v>352</v>
       </c>
@@ -6873,11 +6557,11 @@
       <c r="C39" s="60" t="s">
         <v>365</v>
       </c>
-      <c r="O39" s="59" t="s">
+      <c r="O39" s="63" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="59" t="s">
         <v>352</v>
       </c>
@@ -6887,7 +6571,7 @@
       <c r="C40" s="60" t="s">
         <v>367</v>
       </c>
-      <c r="O40" s="59" t="s">
+      <c r="O40" s="63" t="s">
         <v>345</v>
       </c>
     </row>
@@ -6905,7 +6589,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="59" t="s">
         <v>237</v>
       </c>
@@ -6915,11 +6599,11 @@
       <c r="C42" s="60" t="s">
         <v>371</v>
       </c>
-      <c r="O42" s="59" t="s">
+      <c r="O42" s="63" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="59" t="s">
         <v>237</v>
       </c>
@@ -6929,11 +6613,11 @@
       <c r="C43" s="60" t="s">
         <v>373</v>
       </c>
-      <c r="O43" s="59" t="s">
+      <c r="O43" s="63" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="59" t="s">
         <v>237</v>
       </c>
@@ -6943,11 +6627,11 @@
       <c r="C44" s="60" t="s">
         <v>375</v>
       </c>
-      <c r="O44" s="59" t="s">
+      <c r="O44" s="63" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="59" t="s">
         <v>237</v>
       </c>
@@ -6957,7 +6641,7 @@
       <c r="C45" s="60" t="s">
         <v>376</v>
       </c>
-      <c r="O45" s="59" t="s">
+      <c r="O45" s="63" t="s">
         <v>377</v>
       </c>
     </row>
@@ -6966,33 +6650,33 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="O2" r:id="rId1" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
-    <hyperlink ref="O5" r:id="rId2" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
-    <hyperlink ref="O8" r:id="rId3" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
-    <hyperlink ref="O9" r:id="rId4" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
-    <hyperlink ref="O15" r:id="rId5" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
-    <hyperlink ref="O16" r:id="rId6" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
-    <hyperlink ref="O17" r:id="rId7" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
-    <hyperlink ref="O18" r:id="rId8" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
-    <hyperlink ref="O19" r:id="rId9" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
-    <hyperlink ref="O20" r:id="rId10" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
-    <hyperlink ref="O26" r:id="rId11" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
-    <hyperlink ref="O27" r:id="rId12" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
-    <hyperlink ref="O28" r:id="rId13" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
-    <hyperlink ref="O29" r:id="rId14" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
-    <hyperlink ref="O30" r:id="rId15" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
-    <hyperlink ref="O31" r:id="rId16" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
-    <hyperlink ref="O32" r:id="rId17" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
-    <hyperlink ref="O33" r:id="rId18" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
-    <hyperlink ref="O37" r:id="rId19" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
-    <hyperlink ref="O38" r:id="rId20" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
-    <hyperlink ref="O39" r:id="rId21" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
-    <hyperlink ref="O40" r:id="rId22" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
+    <hyperlink ref="O2" r:id="rId1" location="Kraftwerke" display="&lt;sup&gt;a&lt;/sup&gt;Packaging is included; for the THP, only the mass balance was used, production processes and their energy consumption were not considered due to a lack of data; The calculation was performed using the CML-IA Baseline 3.08 method.&#10;&lt;sup&gt;b&lt;/sup&gt;Greenhouse gas potential during the usage phase was calculated based on the emission factors for the German electricity mix from the Federal Environment Agency for the year 2022 (https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke);&#10;&lt;sup&gt;c&lt;/sup&gt;Assumption of operating time: 24h/day."/>
+    <hyperlink ref="O5" r:id="rId2" location="Kraftwerke" display="&lt;sup&gt;a&lt;/sup&gt;Product packaging is included; for the THP, only the mass balance was used, production processes and their energy consumption were not considered due to a lack of data; the calculation was performed using the CML-IA Baseline 3.08 method.&#10;&lt;sup&gt;b&lt;/sup&gt;Greenhouse gas potential during the usage phase was calculated based on the emission factors for the German electricity mix from the Federal Environment Agency for the year 2022 (https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke);&#10;&lt;sup&gt;c&lt;/sup&gt;Assumption of operating time: 24h/day."/>
+    <hyperlink ref="O8" r:id="rId3" location="Kraftwerke" display="&lt;sup&gt;a&lt;/sup&gt;Product packaging is included; for the THP, only the mass balance was used, production processes and their energy consumption were not considered due to a lack of data; the calculation was performed using the CML-IA Baseline 3.08 method.&#10;&lt;sup&gt;b&lt;/sup&gt;Greenhouse gas potential during the usage phase was calculated based on the emission factors for the German electricity mix from the Federal Environment Agency for the year 2022 (https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke);&#10;&lt;sup&gt;c&lt;/sup&gt;Assumption of operating time: 24h/day."/>
+    <hyperlink ref="O9" r:id="rId4" location="Kraftwerke" display="&lt;sup&gt;a&lt;/sup&gt;Product packaging is included; for the THP, only the mass balance was used, production processes and their energy consumption were not considered due to a lack of data; the calculation was performed using the CML-IA Baseline 3.08 method.&#10;&lt;sup&gt;b&lt;/sup&gt;Greenhouse gas potential during the usage phase was calculated based on the emission factors for the German electricity mix from the Federal Environment Agency for the year 2022 (https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke);&#10;&lt;sup&gt;c&lt;/sup&gt;Assumed operating time: 24h/day."/>
+    <hyperlink ref="O15" r:id="rId5" location="Kraftwerke" display="&lt;sup&gt;b&lt;/sup&gt;Greenhouse gas potential during the usage phase was calculated based on the emission factors for the German electricity mix from the Federal Environment Agency for the year 2022 (https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke);&#10;&lt;sup&gt;a&lt;/sup&gt;Assumed operating time: 3,000 hours per year (range: 2,000 to 4,000 hours);&#10;&lt;sup&gt;c&lt;/sup&gt;The circulation pump has a power rating of 50-250W; for the calculation, an effective power of 150W is assumed."/>
+    <hyperlink ref="O16" r:id="rId6" location="Kraftwerke" display="&lt;sup&gt;a&lt;/sup&gt;Product packaging is included; for the THP, only the mass balance was used, production processes and their energy consumption were not considered due to a lack of data; the calculation was performed using the CML-IA Baseline 3.08 method.&#10;&lt;sup&gt;b&lt;/sup&gt;Greenhouse gas potential during the usage phase was calculated based on the emission factors for the German electricity mix from the Federal Environment Agency for the year 2022 (https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke);&#10;The lifespan of the actuator is assumed to be 15 years (typical lifespan of a seal);&#10;&lt;sup&gt;c&lt;/sup&gt;The operating time of the actuator is 876 hours."/>
+    <hyperlink ref="O17" r:id="rId7" location="Kraftwerke" display="&lt;sup&gt;a&lt;/sup&gt;Product packaging is included; for the THP, only the mass balance was used, production processes and their energy consumption were not considered due to a lack of data; the calculation was performed using the CML-IA Baseline 3.08 method.&#10;&lt;sup&gt;b&lt;/sup&gt;Greenhouse gas potential during the usage phase was calculated based on the emission factors for the German electricity mix from the Federal Environment Agency for the year 2022 (https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke)."/>
+    <hyperlink ref="O18" r:id="rId8" location="Kraftwerke" display="&lt;sup&gt;a&lt;/sup&gt;Product packaging is included; for the THP, only the mass balance was used, production processes and their energy consumption were not considered due to a lack of data; the calculation was performed using the CML-IA Baseline 3.08 method.&#10;&lt;sup&gt;b&lt;/sup&gt;Greenhouse gas potential during the usage phase was calculated based on the emission factors for the German electricity mix from the Federal Environment Agency for the year 2022 (https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke).&#10;&lt;sup&gt;c&lt;/sup&gt;An operating time of 12 hours per day is assumed (average daylight time per year)."/>
+    <hyperlink ref="O19" r:id="rId9" location="Kraftwerke" display="&lt;sup&gt;a&lt;/sup&gt;Product packaging is included; for the THP, only the mass balance was used, production processes and their energy consumption were not considered due to a lack of data; the calculation was performed using the CML-IA Baseline 3.08 method.&#10;&lt;sup&gt;b&lt;/sup&gt;Greenhouse gas potential during the usage phase was calculated based on the emission factors for the German electricity mix from the Federal Environment Agency for the year 2022 (https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke).&#10;&lt;sup&gt;c&lt;/sup&gt;An operating time of 16 hours per day is assumed (average wake time)."/>
+    <hyperlink ref="O20" r:id="rId10" location="Kraftwerke" display="&lt;sup&gt;a&lt;/sup&gt;Product packaging is included; for the THP, only the mass balance was used, production processes and their energy consumption were not considered due to a lack of data; the calculation was performed using the CML-IA Baseline 3.08 method.&#10;&lt;sup&gt;b&lt;/sup&gt;Greenhouse gas potential during the usage phase was calculated based on the emission factors for the German electricity mix from the Federal Environment Agency for the year 2022 (https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke).&#10;&lt;sup&gt;c&lt;/sup&gt;An operating time of 24 hours per day is assumed."/>
+    <hyperlink ref="O26" r:id="rId11" location="Kraftwerke" display="&lt;sup&gt;a&lt;/sup&gt;Product packaging is included; for the THP, only the mass balance was used, production processes and their energy consumption were not considered due to a lack of data; the calculation was performed using the CML-IA Baseline 3.08 method.&#10;&lt;sup&gt;b&lt;/sup&gt;Greenhouse gas potential during the usage phase was calculated based on the emission factors for the German electricity mix from the Federal Environment Agency for the year 2022 (https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke)."/>
+    <hyperlink ref="O27" r:id="rId12" location="Kraftwerke" display="&lt;sup&gt;a&lt;/sup&gt;Product packaging is included; for the THP, only the mass balance was used, production processes and their energy consumption were not considered due to a lack of data; the calculation was performed using the CML-IA Baseline 3.08 method.&#10;&lt;sup&gt;b&lt;/sup&gt;Greenhouse gas potential during the usage phase was calculated based on the emission factors for the German electricity mix from the Federal Environment Agency for the year 2022 (https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke).&#10;&lt;sup&gt;c&lt;/sup&gt;It is assumed that the BACnet and DALI interfaces have similar energy consumption values."/>
+    <hyperlink ref="O28" r:id="rId13" location="Kraftwerke" display="&lt;sup&gt;a&lt;/sup&gt;Product packaging is included; for the THP, only the mass balance was used, production processes and their energy consumption were not considered due to a lack of data; the calculation was performed using the CML-IA Baseline 3.08 method.&#10;&lt;sup&gt;b&lt;/sup&gt;Greenhouse gas potential during the usage phase was calculated based on the emission factors for the German electricity mix from the Federal Environment Agency for the year 2022 (https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke)."/>
+    <hyperlink ref="O29" r:id="rId14" location="Kraftwerke" display="&lt;sup&gt;a&lt;/sup&gt;Product packaging is included; for the THP, only the mass balance was used, production processes and their energy consumption were not considered due to a lack of data; the calculation was performed using the CML-IA Baseline 3.08 method.&#10;&lt;sup&gt;b&lt;/sup&gt;Greenhouse gas potential during the usage phase was calculated based on the emission factors for the German electricity mix from the Federal Environment Agency for the year 2022 (https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke)."/>
+    <hyperlink ref="O30" r:id="rId15" location="Kraftwerke" display="&lt;sup&gt;a&lt;/sup&gt;Product packaging is included; for the THP, only the mass balance was used. Production processes and their energy consumption were not considered due to a lack of data; the calculation was performed using the CML-IA Baseline 3.08 method.&#10;&lt;sup&gt;b&lt;/sup&gt;Greenhouse gas potential during the usage phase was calculated based on the emission factors for the German electricity mix from the Federal Environment Agency for the year 2022 (https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke)."/>
+    <hyperlink ref="O31" r:id="rId16" location="Kraftwerke" display="&lt;sup&gt;a&lt;/sup&gt;Product packaging is included; for the THP, only the mass balance was used. Production processes and their energy consumption were not considered due to a lack of data; the calculation was performed using the CML-IA Baseline 3.08 method.&#10;&lt;sup&gt;b&lt;/sup&gt;Greenhouse gas potential during the usage phase was calculated based on the emission factors for the German electricity mix from the Federal Environment Agency for the year 2022 (https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke)."/>
+    <hyperlink ref="O32" r:id="rId17" location="Kraftwerke" display="&lt;sup&gt;a&lt;/sup&gt;Product packaging is included; for the THP, only the mass balance was used. Production processes and their energy consumption were not considered due to a lack of data; the calculation was performed using the CML-IA Baseline 3.08 method.&#10;&lt;sup&gt;b&lt;/sup&gt;Greenhouse gas potential during the usage phase was calculated based on the emission factors for the German electricity mix from the Federal Environment Agency for the year 2022 (https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke)."/>
+    <hyperlink ref="O33" r:id="rId18" location="Kraftwerke" display="&lt;sup&gt;a&lt;/sup&gt;Product packaging is included; for the THP, only the mass balance was used. Production processes and their energy consumption were not considered due to a lack of data; the calculation was performed using the CML-IA Baseline 3.08 method.&#10;&lt;sup&gt;b&lt;/sup&gt;Greenhouse gas potential during the usage phase was calculated based on the emission factors for the German electricity mix from the Federal Environment Agency for the year 2022 (https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke)."/>
+    <hyperlink ref="O37" r:id="rId19" location="Kraftwerke" display="&lt;sup&gt;a&lt;/sup&gt;An operating time of 24 hours per day was assumed.&#10;&lt;sup&gt;b&lt;/sup&gt;Greenhouse gas potential during the usage phase was calculated based on the emission factors for the German electricity mix from the Federal Environment Agency for the year 2022 (https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke).&#10;&lt;sup&gt;c&lt;/sup&gt;For the THP, only the mass balance was used. Production processes and their energy consumption were not considered due to a lack of data; the calculation was performed using the CML-IA Baseline 3.08 method."/>
+    <hyperlink ref="O38" r:id="rId20" location="Kraftwerke" display="&lt;sup&gt;a&lt;/sup&gt;An operating time of 24 hours per day was assumed.&#10;&lt;sup&gt;b&lt;/sup&gt;Greenhouse gas potential during the usage phase was calculated based on the emission factors for the German electricity mix from the Federal Environment Agency for the year 2022 (https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke).&#10;&lt;sup&gt;c&lt;/sup&gt;For the THP, only the mass balance was used. Production processes and their energy consumption were not considered due to a lack of data; the calculation was performed using the CML-IA Baseline 3.08 method.&#10;&lt;sup&gt;d&lt;/sup&gt;For the average power consumption, the upper value of the manufacturer’s specification in Source [2] was used."/>
+    <hyperlink ref="O39" r:id="rId21" location="Kraftwerke" display="&lt;sup&gt;a&lt;/sup&gt;Product packaging is included; for the THP, only the mass balance was used. Production processes and their energy consumption were not considered due to a lack of data; the calculation was performed using the CML-IA Baseline 3.08 method.&#10;&lt;sup&gt;b&lt;/sup&gt;Greenhouse gas potential during the usage phase was calculated based on the emission factors for the German electricity mix from the Federal Environment Agency for the year 2022 (https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke)."/>
+    <hyperlink ref="O40" r:id="rId22" location="Kraftwerke" display="&lt;sup&gt;a&lt;/sup&gt;Product packaging is included; for the THP, only the mass balance was used. Production processes and their energy consumption were not considered due to a lack of data; the calculation was performed using the CML-IA Baseline 3.08 method.&#10;&lt;sup&gt;b&lt;/sup&gt;Greenhouse gas potential during the usage phase was calculated based on the emission factors for the German electricity mix from the Federal Environment Agency for the year 2022 (https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke)."/>
     <hyperlink ref="O41" r:id="rId23" location="Kraftwerke" display="&lt;sup&gt;b&lt;/sup&gt; Greenhouse gas potential during the usage phase was calculated based on emission factors for the German electricity mix provided by the Federal Environment Agency for the year 2022 (https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke);"/>
-    <hyperlink ref="O42" r:id="rId24" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
-    <hyperlink ref="O43" r:id="rId25" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
-    <hyperlink ref="O44" r:id="rId26" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
-    <hyperlink ref="O45" r:id="rId27" location="Kraftwerke" display="https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke"/>
+    <hyperlink ref="O42" r:id="rId24" location="Kraftwerke" display="&lt;sup&gt;b&lt;/sup&gt;Greenhouse gas potential during the usage phase was calculated based on the emission factors for the German electricity mix from the Federal Environment Agency for the year 2022 (https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke).&#10;&lt;sup&gt;a&lt;/sup&gt;An operating time of 24 hours per day was assumed.&#10;&lt;sup&gt;c&lt;/sup&gt;The router's power consumption is 105W with an effective data transfer rate of 25 Mbit/s."/>
+    <hyperlink ref="O43" r:id="rId25" location="Kraftwerke" display="&lt;sup&gt;a&lt;/sup&gt;An operating time of 24 hours per day is assumed for the measurement computer in its function.&#10;&lt;sup&gt;b&lt;/sup&gt;Greenhouse gas potential during the usage phase was calculated based on the emission factors for the German electricity mix from the Federal Environment Agency for the year 2022 (https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke)."/>
+    <hyperlink ref="O44" r:id="rId26" location="Kraftwerke" display="&lt;sup&gt;a&lt;/sup&gt;An operating time of 24 hours per day is assumed for the measurement computer in its function.&#10;&lt;sup&gt;b&lt;/sup&gt;Greenhouse gas potential during the usage phase was calculated based on the emission factors for the German electricity mix from the Federal Environment Agency for the year 2022 (https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke)."/>
+    <hyperlink ref="O45" r:id="rId27" location="Kraftwerke" display="&lt;sup&gt;b&lt;/sup&gt;Greenhouse gas potential during the usage phase was calculated based on the emission factors for the German electricity mix from the Federal Environment Agency for the year 2022 (https://www.umweltbundesamt.de/themen/klima-energie/energieversorgung/strom-waermeversorgung-in-zahlen?sprungmarke=Strommix#Kraftwerke).&#10;&lt;sup&gt;a&lt;/sup&gt;The monitor of the measurement computer is used only during working hours: 250 days/year * 8 hours = 2000 hours."/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>